<commit_message>
updated more columns for q3 and q4 fy24 MSFT
</commit_message>
<xml_diff>
--- a/MSFT.xlsx
+++ b/MSFT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f922bae05200f16/Documents/Stocks/martinshkreli/models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f922bae05200f16/Documents/Stocks/jukkamic/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="13_ncr:1_{C09E0527-82C7-4143-98EC-0CAA14AC6C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2A312B5-C8DF-41A6-9319-1CCFE6644E1C}"/>
+  <xr:revisionPtr revIDLastSave="152" documentId="13_ncr:1_{C09E0527-82C7-4143-98EC-0CAA14AC6C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E48CC5F5-0BAF-42E9-850E-7EDDCF72323C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AF5D6250-CC2E-478D-A72E-6EAEA79B8F65}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{AF5D6250-CC2E-478D-A72E-6EAEA79B8F65}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -1844,7 +1844,7 @@
     <numFmt numFmtId="166" formatCode="0\x"/>
     <numFmt numFmtId="167" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -1920,12 +1920,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2938,10 +2932,10 @@
   <dimension ref="A1:DS124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C104" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="R79" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="T83" sqref="T83"/>
+      <selection pane="bottomRight" activeCell="U96" sqref="U96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6177,7 +6171,7 @@
         <v>171008</v>
       </c>
       <c r="BH35" s="5">
-        <f t="shared" ref="BG35:BM35" si="39">+BH31*0.67</f>
+        <f t="shared" ref="BH35:BM35" si="39">+BH31*0.67</f>
         <v>177617.06030000004</v>
       </c>
       <c r="BI35" s="5">
@@ -7353,7 +7347,7 @@
         <v>-506</v>
       </c>
       <c r="U41" s="4">
-        <f t="shared" ref="U41:V41" si="86">T41</f>
+        <f t="shared" ref="U41" si="86">T41</f>
         <v>-506</v>
       </c>
       <c r="V41" s="4">
@@ -7480,7 +7474,7 @@
         <v>-227</v>
       </c>
       <c r="BH41" s="5">
-        <f t="shared" ref="BF41:BM41" si="88">+BG61*$BP$49</f>
+        <f t="shared" ref="BH41:BM41" si="88">+BG61*$BP$49</f>
         <v>2256.5426000000002</v>
       </c>
       <c r="BI41" s="5">
@@ -7812,7 +7806,7 @@
         <v>4656</v>
       </c>
       <c r="U43" s="4">
-        <f t="shared" ref="U43:V43" si="103">U42*0.2</f>
+        <f t="shared" ref="U43" si="103">U42*0.2</f>
         <v>5415</v>
       </c>
       <c r="V43" s="4">
@@ -8742,7 +8736,7 @@
         <v>7468</v>
       </c>
       <c r="U46" s="4">
-        <f t="shared" ref="U46:V46" si="136">T46</f>
+        <f t="shared" ref="U46" si="136">T46</f>
         <v>7468</v>
       </c>
       <c r="V46" s="4">
@@ -9232,6 +9226,14 @@
       <c r="T50" s="18">
         <f>T76/P76-1</f>
         <v>0.16171200726795543</v>
+      </c>
+      <c r="U50" s="18">
+        <f t="shared" ref="U50:V50" si="149">U76/Q76-1</f>
+        <v>0.13211787581121692</v>
+      </c>
+      <c r="V50" s="18">
+        <f t="shared" si="149"/>
+        <v>0.11839146674595358</v>
       </c>
       <c r="BA50" s="10"/>
       <c r="BB50" s="10"/>
@@ -9258,60 +9260,68 @@
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
       <c r="G51" s="12">
-        <f t="shared" ref="G51:J53" si="149">G25/C25-1</f>
+        <f t="shared" ref="G51:J53" si="150">G25/C25-1</f>
         <v>0.11212422135957389</v>
       </c>
       <c r="H51" s="12">
-        <f t="shared" si="149"/>
+        <f t="shared" si="150"/>
         <v>0.12912227295788936</v>
       </c>
       <c r="I51" s="12">
-        <f t="shared" si="149"/>
+        <f t="shared" si="150"/>
         <v>0.15404922081239891</v>
       </c>
       <c r="J51" s="12">
-        <f t="shared" si="149"/>
+        <f t="shared" si="150"/>
         <v>0.25008509189925121</v>
       </c>
       <c r="K51" s="12">
-        <f t="shared" ref="K51:K53" si="150">K25/G25-1</f>
+        <f t="shared" ref="K51:K53" si="151">K25/G25-1</f>
         <v>0.22079714262521311</v>
       </c>
       <c r="L51" s="12">
-        <f t="shared" ref="L51:L53" si="151">L25/H25-1</f>
+        <f t="shared" ref="L51:L53" si="152">L25/H25-1</f>
         <v>0.19343967647719618</v>
       </c>
       <c r="M51" s="12">
-        <f t="shared" ref="M51:M53" si="152">M25/I25-1</f>
+        <f t="shared" ref="M51:M53" si="153">M25/I25-1</f>
         <v>0.16506788665879579</v>
       </c>
       <c r="N51" s="12">
-        <f t="shared" ref="N51" si="153">N25/J25-1</f>
+        <f t="shared" ref="N51" si="154">N25/J25-1</f>
         <v>0.12994350282485878</v>
       </c>
       <c r="O51" s="12">
-        <f t="shared" ref="O51" si="154">O25/K25-1</f>
+        <f t="shared" ref="O51" si="155">O25/K25-1</f>
         <v>9.4820134317441296E-2</v>
       </c>
       <c r="P51" s="12">
-        <f t="shared" ref="P51" si="155">P25/L25-1</f>
+        <f t="shared" ref="P51" si="156">P25/L25-1</f>
         <v>6.6892570281124497E-2</v>
       </c>
       <c r="Q51" s="12">
-        <f t="shared" ref="Q51:T51" si="156">Q25/M25-1</f>
+        <f t="shared" ref="Q51:T51" si="157">Q25/M25-1</f>
         <v>0.10937994806510853</v>
       </c>
       <c r="R51" s="12">
-        <f t="shared" si="156"/>
+        <f t="shared" si="157"/>
         <v>0.10186746987951811</v>
       </c>
       <c r="S51" s="12">
-        <f t="shared" si="156"/>
+        <f t="shared" si="157"/>
         <v>0.12918311569996965</v>
       </c>
       <c r="T51" s="12">
-        <f t="shared" si="156"/>
+        <f t="shared" si="157"/>
         <v>0.13216092224444176</v>
+      </c>
+      <c r="U51" s="12">
+        <f t="shared" ref="U51:U53" si="158">U25/Q25-1</f>
+        <v>0.11726421557433198</v>
+      </c>
+      <c r="V51" s="12">
+        <f t="shared" ref="V51:V53" si="159">V25/R25-1</f>
+        <v>0.1107648570335138</v>
       </c>
       <c r="BA51" s="10"/>
       <c r="BB51" s="10"/>
@@ -9338,60 +9348,68 @@
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
       <c r="G52" s="12">
-        <f t="shared" si="149"/>
+        <f t="shared" si="150"/>
         <v>0.19741816505301979</v>
       </c>
       <c r="H52" s="12">
-        <f t="shared" si="149"/>
+        <f t="shared" si="150"/>
         <v>0.23017945909512183</v>
       </c>
       <c r="I52" s="12">
-        <f t="shared" si="149"/>
+        <f t="shared" si="150"/>
         <v>0.23100724696685937</v>
       </c>
       <c r="J52" s="12">
-        <f t="shared" si="149"/>
+        <f t="shared" si="150"/>
         <v>0.29945404233041661</v>
       </c>
       <c r="K52" s="12">
-        <f t="shared" si="150"/>
+        <f t="shared" si="151"/>
         <v>0.30232558139534893</v>
       </c>
       <c r="L52" s="12">
-        <f t="shared" si="151"/>
+        <f t="shared" si="152"/>
         <v>0.25518800082186144</v>
       </c>
       <c r="M52" s="12">
-        <f t="shared" si="152"/>
+        <f t="shared" si="153"/>
         <v>0.25592009525069459</v>
       </c>
       <c r="N52" s="12">
-        <f t="shared" ref="N52:Q52" si="157">N26/J26-1</f>
+        <f t="shared" ref="N52:Q52" si="160">N26/J26-1</f>
         <v>0.19735251798561149</v>
       </c>
       <c r="O52" s="12">
-        <f t="shared" si="157"/>
+        <f t="shared" si="160"/>
         <v>0.20180936613055822</v>
       </c>
       <c r="P52" s="12">
-        <f t="shared" si="157"/>
+        <f t="shared" si="160"/>
         <v>0.17356905112675292</v>
       </c>
       <c r="Q52" s="12">
-        <f t="shared" si="157"/>
+        <f t="shared" si="160"/>
         <v>0.16295359983146374</v>
       </c>
       <c r="R52" s="12">
-        <f t="shared" ref="R52:T53" si="158">R26/N26-1</f>
+        <f t="shared" ref="R52:T53" si="161">R26/N26-1</f>
         <v>0.15328782926360307</v>
       </c>
       <c r="S52" s="12">
+        <f t="shared" si="161"/>
+        <v>0.19355473554735547</v>
+      </c>
+      <c r="T52" s="12">
+        <f t="shared" si="161"/>
+        <v>0.20327320066951837</v>
+      </c>
+      <c r="U52" s="12">
         <f t="shared" si="158"/>
-        <v>0.19355473554735547</v>
-      </c>
-      <c r="T52" s="12">
-        <f t="shared" si="158"/>
-        <v>0.20327320066951837</v>
+        <v>0.20954666908201625</v>
+      </c>
+      <c r="V52" s="12">
+        <f t="shared" si="159"/>
+        <v>0.1884716375609552</v>
       </c>
       <c r="BA52" s="10"/>
       <c r="BB52" s="10"/>
@@ -9418,60 +9436,68 @@
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
       <c r="G53" s="12">
-        <f t="shared" si="149"/>
+        <f t="shared" si="150"/>
         <v>6.4313302793496785E-2</v>
       </c>
       <c r="H53" s="12">
-        <f t="shared" si="149"/>
+        <f t="shared" si="150"/>
         <v>0.14465218378623868</v>
       </c>
       <c r="I53" s="12">
-        <f t="shared" si="149"/>
+        <f t="shared" si="150"/>
         <v>0.18541420387378382</v>
       </c>
       <c r="J53" s="12">
-        <f t="shared" si="149"/>
+        <f t="shared" si="150"/>
         <v>9.1092176607281194E-2</v>
       </c>
       <c r="K53" s="12">
-        <f t="shared" si="150"/>
+        <f t="shared" si="151"/>
         <v>0.12802768166089962</v>
       </c>
       <c r="L53" s="12">
-        <f t="shared" si="151"/>
+        <f t="shared" si="152"/>
         <v>0.15493982277476515</v>
       </c>
       <c r="M53" s="12">
-        <f t="shared" si="152"/>
+        <f t="shared" si="153"/>
         <v>0.11874808223381406</v>
       </c>
       <c r="N53" s="12">
-        <f t="shared" ref="N53:Q53" si="159">N27/J27-1</f>
+        <f t="shared" ref="N53:Q53" si="162">N27/J27-1</f>
         <v>2.6622178049126699E-2</v>
       </c>
       <c r="O53" s="12">
+        <f t="shared" si="162"/>
+        <v>-2.5437677689660321E-3</v>
+      </c>
+      <c r="P53" s="12">
+        <f t="shared" si="162"/>
+        <v>-0.18482679645004296</v>
+      </c>
+      <c r="Q53" s="12">
+        <f t="shared" si="162"/>
+        <v>-9.0784421283598427E-2</v>
+      </c>
+      <c r="R53" s="12">
+        <f t="shared" si="161"/>
+        <v>-3.8448240094046016E-2</v>
+      </c>
+      <c r="S53" s="12">
+        <f t="shared" si="161"/>
+        <v>2.5052505250525048E-2</v>
+      </c>
+      <c r="T53" s="12">
+        <f t="shared" si="161"/>
+        <v>0.1864156774601391</v>
+      </c>
+      <c r="U53" s="12">
+        <f t="shared" si="158"/>
+        <v>0.17496229260935148</v>
+      </c>
+      <c r="V53" s="12">
         <f t="shared" si="159"/>
-        <v>-2.5437677689660321E-3</v>
-      </c>
-      <c r="P53" s="12">
-        <f t="shared" si="159"/>
-        <v>-0.18482679645004296</v>
-      </c>
-      <c r="Q53" s="12">
-        <f t="shared" si="159"/>
-        <v>-9.0784421283598427E-2</v>
-      </c>
-      <c r="R53" s="12">
-        <f t="shared" si="158"/>
-        <v>-3.8448240094046016E-2</v>
-      </c>
-      <c r="S53" s="12">
-        <f t="shared" si="158"/>
-        <v>2.5052505250525048E-2</v>
-      </c>
-      <c r="T53" s="12">
-        <f t="shared" si="158"/>
-        <v>0.1864156774601391</v>
+        <v>0.14311398777418205</v>
       </c>
       <c r="BA53" s="10"/>
       <c r="BB53" s="10"/>
@@ -9494,27 +9520,27 @@
         <v>22</v>
       </c>
       <c r="C54" s="9">
-        <f t="shared" ref="C54:D54" si="160">C35/C31</f>
+        <f t="shared" ref="C54:D54" si="163">C35/C31</f>
         <v>0.6851913477537438</v>
       </c>
       <c r="D54" s="9">
-        <f t="shared" si="160"/>
+        <f t="shared" si="163"/>
         <v>0.66514929821709212</v>
       </c>
       <c r="E54" s="9">
-        <f t="shared" ref="E54:F54" si="161">E35/E31</f>
+        <f t="shared" ref="E54:F54" si="164">E35/E31</f>
         <v>0.68661660146769077</v>
       </c>
       <c r="F54" s="9">
-        <f t="shared" si="161"/>
+        <f t="shared" si="164"/>
         <v>0.67557121447164303</v>
       </c>
       <c r="G54" s="9">
-        <f t="shared" ref="G54:H54" si="162">G35/G31</f>
+        <f t="shared" ref="G54:H54" si="165">G35/G31</f>
         <v>0.70388114334930285</v>
       </c>
       <c r="H54" s="9">
-        <f t="shared" si="162"/>
+        <f t="shared" si="165"/>
         <v>0.67048936762930633</v>
       </c>
       <c r="I54" s="9">
@@ -9522,27 +9548,27 @@
         <v>0.68721526878626582</v>
       </c>
       <c r="J54" s="9">
-        <f t="shared" ref="J54:M54" si="163">J35/J31</f>
+        <f t="shared" ref="J54:M54" si="166">J35/J31</f>
         <v>0.69684954064829263</v>
       </c>
       <c r="K54" s="9">
-        <f t="shared" si="163"/>
+        <f t="shared" si="166"/>
         <v>0.6988768012004325</v>
       </c>
       <c r="L54" s="9">
-        <f t="shared" si="163"/>
+        <f t="shared" si="166"/>
         <v>0.67213114754098358</v>
       </c>
       <c r="M54" s="9">
-        <f t="shared" si="163"/>
+        <f t="shared" si="166"/>
         <v>0.68365072933549431</v>
       </c>
       <c r="N54" s="9">
-        <f t="shared" ref="N54:O54" si="164">N35/N31</f>
+        <f t="shared" ref="N54:O54" si="167">N35/N31</f>
         <v>0.68323532247180174</v>
       </c>
       <c r="O54" s="9">
-        <f t="shared" si="164"/>
+        <f t="shared" si="167"/>
         <v>0.69171222217788597</v>
       </c>
       <c r="P54" s="9">
@@ -9550,193 +9576,193 @@
         <v>0.66845507801391546</v>
       </c>
       <c r="Q54" s="9">
-        <f t="shared" ref="Q54:R54" si="165">Q35/Q31</f>
+        <f t="shared" ref="Q54:R54" si="168">Q35/Q31</f>
         <v>0.69487485101311086</v>
       </c>
       <c r="R54" s="9">
-        <f t="shared" si="165"/>
+        <f t="shared" si="168"/>
         <v>0.70109807969531401</v>
       </c>
       <c r="S54" s="9">
-        <f t="shared" ref="S54:V54" si="166">S35/S31</f>
+        <f t="shared" ref="S54:V54" si="169">S35/S31</f>
         <v>0.71155581506449384</v>
       </c>
       <c r="T54" s="9">
-        <f t="shared" si="166"/>
+        <f t="shared" si="169"/>
         <v>0.68360206385037081</v>
       </c>
       <c r="U54" s="9">
-        <f t="shared" si="166"/>
+        <f t="shared" si="169"/>
         <v>0.70084710142584628</v>
       </c>
       <c r="V54" s="9">
-        <f t="shared" si="166"/>
+        <f t="shared" si="169"/>
         <v>0.69589197707293715</v>
       </c>
       <c r="W54" s="9"/>
       <c r="X54" s="9"/>
       <c r="Y54" s="9">
-        <f t="shared" ref="Y54:AD54" si="167">Y35/Y31</f>
+        <f t="shared" ref="Y54:AD54" si="170">Y35/Y31</f>
         <v>0.78613693998309386</v>
       </c>
       <c r="Z54" s="9">
-        <f t="shared" si="167"/>
+        <f t="shared" si="170"/>
         <v>0.8035811177428106</v>
       </c>
       <c r="AA54" s="9">
-        <f t="shared" si="167"/>
+        <f t="shared" si="170"/>
         <v>0.8307357738310982</v>
       </c>
       <c r="AB54" s="9">
-        <f t="shared" si="167"/>
+        <f t="shared" si="170"/>
         <v>0.83133493205435649</v>
       </c>
       <c r="AC54" s="9">
-        <f t="shared" si="167"/>
+        <f t="shared" si="170"/>
         <v>0.83587868358786832</v>
       </c>
       <c r="AD54" s="9">
-        <f t="shared" si="167"/>
+        <f t="shared" si="170"/>
         <v>0.85228229745662798</v>
       </c>
       <c r="AE54" s="9">
-        <f t="shared" ref="AE54:AM54" si="168">AE35/AE31</f>
+        <f t="shared" ref="AE54:AM54" si="171">AE35/AE31</f>
         <v>0.86299158113251062</v>
       </c>
       <c r="AF54" s="9">
-        <f t="shared" si="168"/>
+        <f t="shared" si="171"/>
         <v>0.90447261841873572</v>
       </c>
       <c r="AG54" s="9">
-        <f t="shared" si="168"/>
+        <f t="shared" si="171"/>
         <v>0.91735708367854185</v>
       </c>
       <c r="AH54" s="9">
-        <f t="shared" si="168"/>
+        <f t="shared" si="171"/>
         <v>0.85749734136830913</v>
       </c>
       <c r="AI54" s="9">
-        <f t="shared" si="168"/>
+        <f t="shared" si="171"/>
         <v>0.86922808851716327</v>
       </c>
       <c r="AJ54" s="9">
-        <f t="shared" si="168"/>
+        <f t="shared" si="171"/>
         <v>0.86341714104996836</v>
       </c>
       <c r="AK54" s="9">
-        <f t="shared" si="168"/>
+        <f t="shared" si="171"/>
         <v>0.8169927727833598</v>
       </c>
       <c r="AL54" s="9">
-        <f t="shared" si="168"/>
+        <f t="shared" si="171"/>
         <v>0.82334482865753256</v>
       </c>
       <c r="AM54" s="9">
-        <f t="shared" si="168"/>
+        <f t="shared" si="171"/>
         <v>0.81767340844305691</v>
       </c>
       <c r="AN54" s="9">
-        <f t="shared" ref="AN54:AW54" si="169">AN35/AN31</f>
+        <f t="shared" ref="AN54:AW54" si="172">AN35/AN31</f>
         <v>0.84417412285111093</v>
       </c>
       <c r="AO54" s="9">
-        <f t="shared" si="169"/>
+        <f t="shared" si="172"/>
         <v>0.82724357526760306</v>
       </c>
       <c r="AP54" s="9">
-        <f t="shared" si="169"/>
+        <f t="shared" si="172"/>
         <v>0.79083369195258402</v>
       </c>
       <c r="AQ54" s="9">
-        <f t="shared" si="169"/>
+        <f t="shared" si="172"/>
         <v>0.80804369414101296</v>
       </c>
       <c r="AR54" s="9">
-        <f t="shared" si="169"/>
+        <f t="shared" si="172"/>
         <v>0.79199822030562828</v>
       </c>
       <c r="AS54" s="9">
-        <f t="shared" si="169"/>
+        <f t="shared" si="172"/>
         <v>0.80162921707957235</v>
       </c>
       <c r="AT54" s="9">
-        <f t="shared" si="169"/>
+        <f t="shared" si="172"/>
         <v>0.77729007906438097</v>
       </c>
       <c r="AU54" s="9">
-        <f t="shared" si="169"/>
+        <f t="shared" si="172"/>
         <v>0.76221803236439101</v>
       </c>
       <c r="AV54" s="9">
-        <f t="shared" si="169"/>
+        <f t="shared" si="172"/>
         <v>0.7398938971598864</v>
       </c>
       <c r="AW54" s="9">
-        <f t="shared" si="169"/>
+        <f t="shared" si="172"/>
         <v>0.68981838701876019</v>
       </c>
       <c r="AX54" s="9">
-        <f t="shared" ref="AX54:AY54" si="170">AX35/AX31</f>
+        <f t="shared" ref="AX54:AY54" si="173">AX35/AX31</f>
         <v>0.64695447745244705</v>
       </c>
       <c r="AY54" s="9">
-        <f t="shared" si="170"/>
+        <f t="shared" si="173"/>
         <v>0.61579934364744493</v>
       </c>
       <c r="AZ54" s="9">
-        <f t="shared" ref="AZ54:BA54" si="171">AZ35/AZ31</f>
+        <f t="shared" ref="AZ54:BA54" si="174">AZ35/AZ31</f>
         <v>0.64522475691460168</v>
       </c>
       <c r="BA54" s="9">
-        <f t="shared" si="171"/>
+        <f t="shared" si="174"/>
         <v>0.65247372236317502</v>
       </c>
       <c r="BB54" s="9">
-        <f t="shared" ref="BB54:BF54" si="172">BB35/BB31</f>
+        <f t="shared" ref="BB54:BF54" si="175">BB35/BB31</f>
         <v>0.65901957200638894</v>
       </c>
       <c r="BC54" s="9">
-        <f t="shared" si="172"/>
+        <f t="shared" si="175"/>
         <v>0.67781001992797962</v>
       </c>
       <c r="BD54" s="9">
-        <f t="shared" si="172"/>
+        <f t="shared" si="175"/>
         <v>0.68925800771024703</v>
       </c>
       <c r="BE54" s="9">
-        <f t="shared" si="172"/>
+        <f t="shared" si="175"/>
         <v>0.68401674484289099</v>
       </c>
       <c r="BF54" s="9">
-        <f t="shared" si="172"/>
+        <f t="shared" si="175"/>
         <v>0.68920085883491022</v>
       </c>
       <c r="BG54" s="9">
-        <f t="shared" ref="BG54:BM54" si="173">BG35/BG31</f>
+        <f t="shared" ref="BG54:BM54" si="176">BG35/BG31</f>
         <v>0.69764443827971379</v>
       </c>
       <c r="BH54" s="9">
-        <f t="shared" si="173"/>
+        <f t="shared" si="176"/>
         <v>0.67</v>
       </c>
       <c r="BI54" s="9">
-        <f t="shared" si="173"/>
+        <f t="shared" si="176"/>
         <v>0.67</v>
       </c>
       <c r="BJ54" s="9">
-        <f t="shared" si="173"/>
+        <f t="shared" si="176"/>
         <v>0.67</v>
       </c>
       <c r="BK54" s="9">
-        <f t="shared" si="173"/>
+        <f t="shared" si="176"/>
         <v>0.67</v>
       </c>
       <c r="BL54" s="9">
-        <f t="shared" si="173"/>
+        <f t="shared" si="176"/>
         <v>0.67</v>
       </c>
       <c r="BM54" s="9">
-        <f t="shared" si="173"/>
+        <f t="shared" si="176"/>
         <v>0.67</v>
       </c>
       <c r="BO54" t="s">
@@ -9752,63 +9778,63 @@
         <v>455</v>
       </c>
       <c r="C55" s="9">
-        <f t="shared" ref="C55" si="174">+C40/C31</f>
+        <f t="shared" ref="C55" si="177">+C40/C31</f>
         <v>0.38378460142187265</v>
       </c>
       <c r="D55" s="9">
-        <f t="shared" ref="D55:E55" si="175">+D40/D31</f>
+        <f t="shared" ref="D55:E55" si="178">+D40/D31</f>
         <v>0.37638866309001245</v>
       </c>
       <c r="E55" s="9">
-        <f t="shared" si="175"/>
+        <f t="shared" si="178"/>
         <v>0.37049199051997372</v>
       </c>
       <c r="F55" s="9">
-        <f t="shared" ref="F55:I55" si="176">+F40/F31</f>
+        <f t="shared" ref="F55:I55" si="179">+F40/F31</f>
         <v>0.35250966266137301</v>
       </c>
       <c r="G55" s="9">
-        <f t="shared" si="176"/>
+        <f t="shared" si="179"/>
         <v>0.42730257845723207</v>
       </c>
       <c r="H55" s="9">
-        <f t="shared" si="176"/>
+        <f t="shared" si="179"/>
         <v>0.41547497446373849</v>
       </c>
       <c r="I55" s="9">
-        <f t="shared" si="176"/>
+        <f t="shared" si="179"/>
         <v>0.40876612477820939</v>
       </c>
       <c r="J55" s="9">
-        <f t="shared" ref="J55:Q55" si="177">+J40/J31</f>
+        <f t="shared" ref="J55:Q55" si="180">+J40/J31</f>
         <v>0.41374154966198645</v>
       </c>
       <c r="K55" s="9">
-        <f t="shared" si="177"/>
+        <f t="shared" si="180"/>
         <v>0.44658737339188381</v>
       </c>
       <c r="L55" s="9">
-        <f t="shared" si="177"/>
+        <f t="shared" si="180"/>
         <v>0.43007655428394681</v>
       </c>
       <c r="M55" s="9">
-        <f t="shared" si="177"/>
+        <f t="shared" si="180"/>
         <v>0.41256077795786061</v>
       </c>
       <c r="N55" s="9">
-        <f t="shared" si="177"/>
+        <f t="shared" si="180"/>
         <v>0.3959124650535043</v>
       </c>
       <c r="O55" s="9">
-        <f t="shared" si="177"/>
+        <f t="shared" si="180"/>
         <v>0.42931247755476637</v>
       </c>
       <c r="P55" s="9">
-        <f t="shared" si="177"/>
+        <f t="shared" si="180"/>
         <v>0.3867328947617874</v>
       </c>
       <c r="Q55" s="9">
-        <f t="shared" si="177"/>
+        <f t="shared" si="180"/>
         <v>0.42287681858599618</v>
       </c>
       <c r="R55" s="9">
@@ -9816,19 +9842,19 @@
         <v>0.4316503230169606</v>
       </c>
       <c r="S55" s="9">
-        <f t="shared" ref="S55:V55" si="178">+S40/S31</f>
+        <f t="shared" ref="S55:V55" si="181">+S40/S31</f>
         <v>0.47587451563246458</v>
       </c>
       <c r="T55" s="9">
-        <f t="shared" si="178"/>
+        <f t="shared" si="181"/>
         <v>0.43585940019348596</v>
       </c>
       <c r="U55" s="9">
-        <f t="shared" si="178"/>
+        <f t="shared" si="181"/>
         <v>0.44587603866921011</v>
       </c>
       <c r="V55" s="9">
-        <f t="shared" si="178"/>
+        <f t="shared" si="181"/>
         <v>0.43142737960974553</v>
       </c>
       <c r="W55" s="9"/>
@@ -9853,59 +9879,59 @@
       <c r="AP55" s="9"/>
       <c r="AQ55" s="9"/>
       <c r="AR55" s="9">
-        <f t="shared" ref="AR55:AT55" si="179">AR40/AR31</f>
+        <f t="shared" ref="AR55:AT55" si="182">AR40/AR31</f>
         <v>0.35410784263394768</v>
       </c>
       <c r="AS55" s="9">
-        <f t="shared" si="179"/>
+        <f t="shared" si="182"/>
         <v>0.38661097240893672</v>
       </c>
       <c r="AT55" s="9">
-        <f t="shared" si="179"/>
+        <f t="shared" si="182"/>
         <v>0.38833049769097694</v>
       </c>
       <c r="AU55" s="9">
-        <f t="shared" ref="AU55:BE55" si="180">AU40/AU31</f>
+        <f t="shared" ref="AU55:BE55" si="183">AU40/AU31</f>
         <v>0.37920323372624554</v>
       </c>
       <c r="AV55" s="9">
-        <f t="shared" si="180"/>
+        <f t="shared" si="183"/>
         <v>0.34379375457616668</v>
       </c>
       <c r="AW55" s="9">
-        <f t="shared" si="180"/>
+        <f t="shared" si="183"/>
         <v>0.32114518673776099</v>
       </c>
       <c r="AX55" s="9">
-        <f t="shared" si="180"/>
+        <f t="shared" si="183"/>
         <v>0.30104723231459712</v>
       </c>
       <c r="AY55" s="9">
-        <f t="shared" si="180"/>
+        <f t="shared" si="183"/>
         <v>0.24955461790904829</v>
       </c>
       <c r="AZ55" s="9">
-        <f t="shared" si="180"/>
+        <f t="shared" si="183"/>
         <v>0.30372472067183731</v>
       </c>
       <c r="BA55" s="9">
-        <f t="shared" si="180"/>
+        <f t="shared" si="183"/>
         <v>0.31766944545125048</v>
       </c>
       <c r="BB55" s="9">
-        <f t="shared" si="180"/>
+        <f t="shared" si="183"/>
         <v>0.3413698020549415</v>
       </c>
       <c r="BC55" s="9">
-        <f t="shared" si="180"/>
+        <f t="shared" si="183"/>
         <v>0.37030381428521486</v>
       </c>
       <c r="BD55" s="9">
-        <f t="shared" si="180"/>
+        <f t="shared" si="183"/>
         <v>0.41594878872971303</v>
       </c>
       <c r="BE55" s="9">
-        <f t="shared" si="180"/>
+        <f t="shared" si="183"/>
         <v>0.4205527815604983</v>
       </c>
       <c r="BF55" s="9">
@@ -9913,31 +9939,31 @@
         <v>0.41772880636104098</v>
       </c>
       <c r="BG55" s="9">
-        <f t="shared" ref="BG55:BM55" si="181">BG40/BG31</f>
+        <f t="shared" ref="BG55:BM55" si="184">BG40/BG31</f>
         <v>0.44644299573273716</v>
       </c>
       <c r="BH55" s="9">
-        <f t="shared" si="181"/>
+        <f t="shared" si="184"/>
         <v>0.43076111479252999</v>
       </c>
       <c r="BI55" s="9">
-        <f t="shared" si="181"/>
+        <f t="shared" si="184"/>
         <v>0.44233942528487596</v>
       </c>
       <c r="BJ55" s="9">
-        <f t="shared" si="181"/>
+        <f t="shared" si="184"/>
         <v>0.45352789822823952</v>
       </c>
       <c r="BK55" s="9">
-        <f t="shared" si="181"/>
+        <f t="shared" si="184"/>
         <v>0.46432293945996628</v>
       </c>
       <c r="BL55" s="9">
-        <f t="shared" si="181"/>
+        <f t="shared" si="184"/>
         <v>0.47472284219397148</v>
       </c>
       <c r="BM55" s="9">
-        <f t="shared" si="181"/>
+        <f t="shared" si="184"/>
         <v>0.48472766619704694</v>
       </c>
       <c r="BP55" s="4"/>
@@ -9947,19 +9973,19 @@
         <v>89</v>
       </c>
       <c r="C56" s="9">
-        <f t="shared" ref="C56:D56" si="182">+C43/C42</f>
+        <f t="shared" ref="C56:D56" si="185">+C43/C42</f>
         <v>0.15828472331704241</v>
       </c>
       <c r="D56" s="9">
-        <f t="shared" si="182"/>
+        <f t="shared" si="185"/>
         <v>0.17294994675186368</v>
       </c>
       <c r="E56" s="9">
-        <f t="shared" ref="E56:F56" si="183">+E43/E42</f>
+        <f t="shared" ref="E56:F56" si="186">+E43/E42</f>
         <v>0.16281242700303666</v>
       </c>
       <c r="F56" s="9">
-        <f t="shared" si="183"/>
+        <f t="shared" si="186"/>
         <v>0.16540008940545373</v>
       </c>
       <c r="G56" s="9">
@@ -9967,35 +9993,35 @@
         <v>0.13836516993301909</v>
       </c>
       <c r="H56" s="9">
-        <f t="shared" ref="H56:O56" si="184">+H43/H42</f>
+        <f t="shared" ref="H56:O56" si="187">+H43/H42</f>
         <v>0.15673228990565524</v>
       </c>
       <c r="I56" s="9">
-        <f t="shared" si="184"/>
+        <f t="shared" si="187"/>
         <v>0.10321420283128337</v>
       </c>
       <c r="J56" s="9">
-        <f t="shared" si="184"/>
+        <f t="shared" si="187"/>
         <v>0.15186807523834064</v>
       </c>
       <c r="K56" s="9">
-        <f t="shared" si="184"/>
+        <f t="shared" si="187"/>
         <v>9.2574546871954783E-4</v>
       </c>
       <c r="L56" s="9">
-        <f t="shared" si="184"/>
+        <f t="shared" si="187"/>
         <v>0.16655562958027981</v>
       </c>
       <c r="M56" s="9">
-        <f t="shared" si="184"/>
+        <f t="shared" si="187"/>
         <v>0.17147102526002972</v>
       </c>
       <c r="N56" s="9">
-        <f t="shared" si="184"/>
+        <f t="shared" si="187"/>
         <v>0.18289647093278666</v>
       </c>
       <c r="O56" s="9">
-        <f t="shared" si="184"/>
+        <f t="shared" si="187"/>
         <v>0.18616725384758021</v>
       </c>
       <c r="P56" s="9">
@@ -10003,193 +10029,193 @@
         <v>0.19243817296818919</v>
       </c>
       <c r="Q56" s="9">
-        <f t="shared" ref="Q56:R56" si="185">+Q43/Q42</f>
+        <f t="shared" ref="Q56:R56" si="188">+Q43/Q42</f>
         <v>0.19291668504388479</v>
       </c>
       <c r="R56" s="9">
-        <f t="shared" si="185"/>
+        <f t="shared" si="188"/>
         <v>0.18789177821814212</v>
       </c>
       <c r="S56" s="9">
-        <f t="shared" ref="S56:V56" si="186">+S43/S42</f>
+        <f t="shared" ref="S56:V56" si="189">+S43/S42</f>
         <v>0.18300102624248643</v>
       </c>
       <c r="T56" s="9">
-        <f t="shared" si="186"/>
+        <f t="shared" si="189"/>
         <v>0.17552589911784663</v>
       </c>
       <c r="U56" s="9">
-        <f t="shared" si="186"/>
+        <f t="shared" si="189"/>
         <v>0.2</v>
       </c>
       <c r="V56" s="9">
-        <f t="shared" si="186"/>
+        <f t="shared" si="189"/>
         <v>0.1913394495412844</v>
       </c>
       <c r="W56" s="9"/>
       <c r="X56" s="9"/>
       <c r="Y56" s="9">
-        <f t="shared" ref="Y56:AD56" si="187">+Y43/Y42</f>
+        <f t="shared" ref="Y56:AD56" si="190">+Y43/Y42</f>
         <v>0.31951219512195123</v>
       </c>
       <c r="Z56" s="9">
-        <f t="shared" si="187"/>
+        <f t="shared" si="190"/>
         <v>0.30998509687034276</v>
       </c>
       <c r="AA56" s="9">
-        <f t="shared" si="187"/>
+        <f t="shared" si="190"/>
         <v>0.31988472622478387</v>
       </c>
       <c r="AB56" s="9">
-        <f t="shared" si="187"/>
+        <f t="shared" si="190"/>
         <v>0.31977159172019987</v>
       </c>
       <c r="AC56" s="9">
-        <f t="shared" si="187"/>
+        <f t="shared" si="190"/>
         <v>0.31788079470198677</v>
       </c>
       <c r="AD56" s="9">
-        <f t="shared" si="187"/>
+        <f t="shared" si="190"/>
         <v>0.32263895164934481</v>
       </c>
       <c r="AE56" s="9">
-        <f t="shared" ref="AE56:AM56" si="188">+AE43/AE42</f>
+        <f t="shared" ref="AE56:AM56" si="191">+AE43/AE42</f>
         <v>0.35039952648712636</v>
       </c>
       <c r="AF56" s="9">
-        <f t="shared" si="188"/>
+        <f t="shared" si="191"/>
         <v>0.35001881821603315</v>
       </c>
       <c r="AG56" s="9">
-        <f t="shared" si="188"/>
+        <f t="shared" si="191"/>
         <v>0.35815459328207205</v>
       </c>
       <c r="AH56" s="9">
-        <f t="shared" si="188"/>
+        <f t="shared" si="191"/>
         <v>0.35001278663370555</v>
       </c>
       <c r="AI56" s="9">
-        <f t="shared" si="188"/>
+        <f t="shared" si="191"/>
         <v>0.34379205326156242</v>
       </c>
       <c r="AJ56" s="9">
-        <f t="shared" si="188"/>
+        <f t="shared" si="191"/>
         <v>0.32557343375556319</v>
       </c>
       <c r="AK56" s="9">
-        <f t="shared" si="188"/>
+        <f t="shared" si="191"/>
         <v>0.31744937526928046</v>
       </c>
       <c r="AL56" s="9">
-        <f t="shared" si="188"/>
+        <f t="shared" si="191"/>
         <v>0.31992699743139108</v>
       </c>
       <c r="AM56" s="9">
-        <f t="shared" si="188"/>
+        <f t="shared" si="191"/>
         <v>0.32959659602323871</v>
       </c>
       <c r="AN56" s="9">
-        <f t="shared" ref="AN56:AW56" si="189">+AN43/AN42</f>
+        <f t="shared" ref="AN56:AW56" si="192">+AN43/AN42</f>
         <v>0.26305027664180902</v>
       </c>
       <c r="AO56" s="9">
-        <f t="shared" si="189"/>
+        <f t="shared" si="192"/>
         <v>0.31009747015660938</v>
       </c>
       <c r="AP56" s="9">
-        <f t="shared" si="189"/>
+        <f t="shared" si="192"/>
         <v>0.30028356798169248</v>
       </c>
       <c r="AQ56" s="9">
-        <f t="shared" si="189"/>
+        <f t="shared" si="192"/>
         <v>0.25753758293440832</v>
       </c>
       <c r="AR56" s="9">
-        <f t="shared" si="189"/>
+        <f t="shared" si="192"/>
         <v>0.26063222668850183</v>
       </c>
       <c r="AS56" s="9">
-        <f t="shared" si="189"/>
+        <f t="shared" si="192"/>
         <v>0.24940172303765157</v>
       </c>
       <c r="AT56" s="9">
-        <f t="shared" si="189"/>
+        <f t="shared" si="192"/>
         <v>0.17530547540166008</v>
       </c>
       <c r="AU56" s="9">
-        <f t="shared" si="189"/>
+        <f t="shared" si="192"/>
         <v>0.18583977512297961</v>
       </c>
       <c r="AV56" s="9">
-        <f t="shared" si="189"/>
+        <f t="shared" si="192"/>
         <v>0.19181576223569421</v>
       </c>
       <c r="AW56" s="9">
-        <f t="shared" si="189"/>
+        <f t="shared" si="192"/>
         <v>0.20560346369914481</v>
       </c>
       <c r="AX56" s="9">
-        <f t="shared" ref="AX56:AY56" si="190">+AX43/AX42</f>
+        <f t="shared" ref="AX56:AY56" si="193">+AX43/AX42</f>
         <v>0.22140402552773686</v>
       </c>
       <c r="AY56" s="9">
-        <f t="shared" si="190"/>
+        <f t="shared" si="193"/>
         <v>0.1415560136139207</v>
       </c>
       <c r="AZ56" s="9">
-        <f t="shared" ref="AZ56:BA56" si="191">+AZ43/AZ42</f>
+        <f t="shared" ref="AZ56:BA56" si="194">+AZ43/AZ42</f>
         <v>0.14605886052901645</v>
       </c>
       <c r="BA56" s="9">
-        <f t="shared" si="191"/>
+        <f t="shared" si="194"/>
         <v>0.5456763722103416</v>
       </c>
       <c r="BB56" s="9">
-        <f t="shared" ref="BB56:BF56" si="192">+BB43/BB42</f>
+        <f t="shared" ref="BB56:BF56" si="195">+BB43/BB42</f>
         <v>0.10181285478850027</v>
       </c>
       <c r="BC56" s="9">
-        <f t="shared" si="192"/>
+        <f t="shared" si="195"/>
         <v>0.16507655177615205</v>
       </c>
       <c r="BD56" s="9">
-        <f t="shared" si="192"/>
+        <f t="shared" si="195"/>
         <v>0.13826615285083402</v>
       </c>
       <c r="BE56" s="9">
-        <f t="shared" si="192"/>
+        <f t="shared" si="195"/>
         <v>0.13113383343685794</v>
       </c>
       <c r="BF56" s="9">
-        <f t="shared" si="192"/>
+        <f t="shared" si="195"/>
         <v>0.15</v>
       </c>
       <c r="BG56" s="9">
-        <f t="shared" ref="BG56:BM56" si="193">+BG43/BG42</f>
+        <f t="shared" ref="BG56:BM56" si="196">+BG43/BG42</f>
         <v>0.19</v>
       </c>
       <c r="BH56" s="9">
-        <f t="shared" si="193"/>
+        <f t="shared" si="196"/>
         <v>0.15</v>
       </c>
       <c r="BI56" s="9">
-        <f t="shared" si="193"/>
+        <f t="shared" si="196"/>
         <v>0.15</v>
       </c>
       <c r="BJ56" s="9">
-        <f t="shared" si="193"/>
+        <f t="shared" si="196"/>
         <v>0.15</v>
       </c>
       <c r="BK56" s="9">
-        <f t="shared" si="193"/>
+        <f t="shared" si="196"/>
         <v>0.15</v>
       </c>
       <c r="BL56" s="9">
-        <f t="shared" si="193"/>
+        <f t="shared" si="196"/>
         <v>0.15</v>
       </c>
       <c r="BM56" s="9">
-        <f t="shared" si="193"/>
+        <f t="shared" si="196"/>
         <v>0.15</v>
       </c>
       <c r="BO56" t="s">
@@ -10205,55 +10231,55 @@
         <v>156</v>
       </c>
       <c r="C57" s="9">
-        <f t="shared" ref="C57" si="194">(C29-C32)/C29</f>
+        <f t="shared" ref="C57" si="197">(C29-C32)/C29</f>
         <v>0.79039827498731607</v>
       </c>
       <c r="D57" s="9">
-        <f t="shared" ref="D57:E57" si="195">(D29-D32)/D29</f>
+        <f t="shared" ref="D57:E57" si="198">(D29-D32)/D29</f>
         <v>0.72796494111202414</v>
       </c>
       <c r="E57" s="9">
-        <f t="shared" si="195"/>
+        <f t="shared" si="198"/>
         <v>0.78728498519311951</v>
       </c>
       <c r="F57" s="9">
-        <f t="shared" ref="F57:I57" si="196">(F29-F32)/F29</f>
+        <f t="shared" ref="F57:I57" si="199">(F29-F32)/F29</f>
         <v>0.75918884664131814</v>
       </c>
       <c r="G57" s="9">
-        <f t="shared" si="196"/>
+        <f t="shared" si="199"/>
         <v>0.77238499019173579</v>
       </c>
       <c r="H57" s="9">
-        <f t="shared" si="196"/>
+        <f t="shared" si="199"/>
         <v>0.68869475847893113</v>
       </c>
       <c r="I57" s="9">
-        <f t="shared" si="196"/>
+        <f t="shared" si="199"/>
         <v>0.74651810584958223</v>
       </c>
       <c r="J57" s="9">
-        <f t="shared" ref="J57:L57" si="197">(J29-J32)/J29</f>
+        <f t="shared" ref="J57:L57" si="200">(J29-J32)/J29</f>
         <v>0.7736297391488014</v>
       </c>
       <c r="K57" s="9">
-        <f t="shared" si="197"/>
+        <f t="shared" si="200"/>
         <v>0.77199206301485179</v>
       </c>
       <c r="L57" s="9">
-        <f t="shared" si="197"/>
+        <f t="shared" si="200"/>
         <v>0.69531738774724483</v>
       </c>
       <c r="M57" s="9">
-        <f t="shared" ref="M57:O57" si="198">(M29-M32)/M29</f>
+        <f t="shared" ref="M57:O57" si="201">(M29-M32)/M29</f>
         <v>0.73603593228146957</v>
       </c>
       <c r="N57" s="9">
-        <f t="shared" si="198"/>
+        <f t="shared" si="201"/>
         <v>0.75735130318556476</v>
       </c>
       <c r="O57" s="9">
-        <f t="shared" si="198"/>
+        <f t="shared" si="201"/>
         <v>0.72670097198399086</v>
       </c>
       <c r="P57" s="9">
@@ -10261,27 +10287,27 @@
         <v>0.65550644790216139</v>
       </c>
       <c r="Q57" s="9">
-        <f t="shared" ref="Q57:V57" si="199">(Q29-Q32)/Q29</f>
+        <f t="shared" ref="Q57:V57" si="202">(Q29-Q32)/Q29</f>
         <v>0.74717731588401337</v>
       </c>
       <c r="R57" s="9">
-        <f t="shared" si="199"/>
+        <f t="shared" si="202"/>
         <v>0.77030795704028954</v>
       </c>
       <c r="S57" s="9">
-        <f t="shared" si="199"/>
+        <f t="shared" si="202"/>
         <v>0.77270679111683294</v>
       </c>
       <c r="T57" s="9">
-        <f t="shared" si="199"/>
+        <f t="shared" si="202"/>
         <v>0.68512750118789922</v>
       </c>
       <c r="U57" s="9">
-        <f t="shared" si="199"/>
+        <f t="shared" si="202"/>
         <v>0.74596018735363001</v>
       </c>
       <c r="V57" s="9">
-        <f t="shared" si="199"/>
+        <f t="shared" si="202"/>
         <v>0.89120072633729286</v>
       </c>
       <c r="W57" s="9"/>
@@ -10313,63 +10339,63 @@
       <c r="AW57" s="9"/>
       <c r="AX57" s="9"/>
       <c r="AY57" s="9">
-        <f t="shared" ref="AY57" si="200">(AY29-AY32)/AY29</f>
+        <f t="shared" ref="AY57" si="203">(AY29-AY32)/AY29</f>
         <v>0.70927774706513613</v>
       </c>
       <c r="AZ57" s="9">
-        <f t="shared" ref="AZ57:BM57" si="201">(AZ29-AZ32)/AZ29</f>
+        <f t="shared" ref="AZ57:BM57" si="204">(AZ29-AZ32)/AZ29</f>
         <v>0.76218833743398473</v>
       </c>
       <c r="BA57" s="9">
-        <f t="shared" si="201"/>
+        <f t="shared" si="204"/>
         <v>0.76091911251686128</v>
       </c>
       <c r="BB57" s="9">
-        <f t="shared" si="201"/>
+        <f t="shared" si="204"/>
         <v>0.75369689264254036</v>
       </c>
       <c r="BC57" s="9">
-        <f t="shared" si="201"/>
+        <f t="shared" si="204"/>
         <v>0.76459781602269217</v>
       </c>
       <c r="BD57" s="9">
-        <f t="shared" si="201"/>
+        <f t="shared" si="204"/>
         <v>0.74366153586402906</v>
       </c>
       <c r="BE57" s="9">
-        <f t="shared" si="201"/>
+        <f t="shared" si="204"/>
         <v>0.73788703734257277</v>
       </c>
       <c r="BF57" s="9">
-        <f t="shared" si="201"/>
+        <f t="shared" si="204"/>
         <v>0.72481800336944935</v>
       </c>
       <c r="BG57" s="9">
-        <f t="shared" si="201"/>
+        <f t="shared" si="204"/>
         <v>0.76422274713229277</v>
       </c>
       <c r="BH57" s="9">
-        <f t="shared" si="201"/>
+        <f t="shared" si="204"/>
         <v>0.75</v>
       </c>
       <c r="BI57" s="9">
-        <f t="shared" si="201"/>
+        <f t="shared" si="204"/>
         <v>0.75</v>
       </c>
       <c r="BJ57" s="9">
-        <f t="shared" si="201"/>
+        <f t="shared" si="204"/>
         <v>0.75</v>
       </c>
       <c r="BK57" s="9">
-        <f t="shared" si="201"/>
+        <f t="shared" si="204"/>
         <v>0.75</v>
       </c>
       <c r="BL57" s="9">
-        <f t="shared" si="201"/>
+        <f t="shared" si="204"/>
         <v>0.75</v>
       </c>
       <c r="BM57" s="9">
-        <f t="shared" si="201"/>
+        <f t="shared" si="204"/>
         <v>0.75</v>
       </c>
       <c r="BP57" s="1"/>
@@ -10379,55 +10405,55 @@
         <v>157</v>
       </c>
       <c r="C58" s="9">
-        <f t="shared" ref="C58" si="202">(C30-C33)/C30</f>
+        <f t="shared" ref="C58" si="205">(C30-C33)/C30</f>
         <v>0.58922890032972752</v>
       </c>
       <c r="D58" s="9">
-        <f t="shared" ref="D58:E58" si="203">(D30-D33)/D30</f>
+        <f t="shared" ref="D58:E58" si="206">(D30-D33)/D30</f>
         <v>0.60366736368023166</v>
       </c>
       <c r="E58" s="9">
-        <f t="shared" si="203"/>
+        <f t="shared" si="206"/>
         <v>0.60318537859007837</v>
       </c>
       <c r="F58" s="9">
-        <f t="shared" ref="F58:K58" si="204">(F30-F33)/F30</f>
+        <f t="shared" ref="F58:K58" si="207">(F30-F33)/F30</f>
         <v>0.59926581514633415</v>
       </c>
       <c r="G58" s="9">
-        <f t="shared" si="204"/>
+        <f t="shared" si="207"/>
         <v>0.65317783710364852</v>
       </c>
       <c r="H58" s="9">
-        <f t="shared" si="204"/>
+        <f t="shared" si="207"/>
         <v>0.65548780487804881</v>
       </c>
       <c r="I58" s="9">
-        <f t="shared" si="204"/>
+        <f t="shared" si="207"/>
         <v>0.64692143518704948</v>
       </c>
       <c r="J58" s="9">
-        <f t="shared" si="204"/>
+        <f t="shared" si="207"/>
         <v>0.64341882854413168</v>
       </c>
       <c r="K58" s="9">
-        <f t="shared" si="204"/>
+        <f t="shared" si="207"/>
         <v>0.65648748518441047</v>
       </c>
       <c r="L58" s="9">
-        <f t="shared" ref="L58:O58" si="205">(L30-L33)/L30</f>
+        <f t="shared" ref="L58:O58" si="208">(L30-L33)/L30</f>
         <v>0.65656402468577335</v>
       </c>
       <c r="M58" s="9">
-        <f t="shared" si="205"/>
+        <f t="shared" si="208"/>
         <v>0.65521660311308372</v>
       </c>
       <c r="N58" s="9">
-        <f t="shared" si="205"/>
+        <f t="shared" si="208"/>
         <v>0.64398832168450859</v>
       </c>
       <c r="O58" s="9">
-        <f t="shared" si="205"/>
+        <f t="shared" si="208"/>
         <v>0.67569296995433525</v>
       </c>
       <c r="P58" s="9">
@@ -10435,27 +10461,27 @@
         <v>0.67435826662986476</v>
       </c>
       <c r="Q58" s="9">
-        <f t="shared" ref="Q58:V58" si="206">(Q30-Q33)/Q30</f>
+        <f t="shared" ref="Q58:V58" si="209">(Q30-Q33)/Q30</f>
         <v>0.67299900721779493</v>
       </c>
       <c r="R58" s="9">
-        <f t="shared" si="206"/>
+        <f t="shared" si="209"/>
         <v>0.67144600366076879</v>
       </c>
       <c r="S58" s="9">
-        <f t="shared" si="206"/>
+        <f t="shared" si="209"/>
         <v>0.68837538431506518</v>
       </c>
       <c r="T58" s="9">
-        <f t="shared" si="206"/>
+        <f t="shared" si="209"/>
         <v>0.68293135866663568</v>
       </c>
       <c r="U58" s="9">
-        <f t="shared" si="206"/>
+        <f t="shared" si="209"/>
         <v>0.68363928714993971</v>
       </c>
       <c r="V58" s="9">
-        <f t="shared" si="206"/>
+        <f t="shared" si="209"/>
         <v>0.64577751892836344</v>
       </c>
       <c r="W58" s="9"/>
@@ -10487,63 +10513,63 @@
       <c r="AW58" s="9"/>
       <c r="AX58" s="9"/>
       <c r="AY58" s="9">
-        <f t="shared" ref="AY58" si="207">(AY30-AY33)/AY30</f>
+        <f t="shared" ref="AY58" si="210">(AY30-AY33)/AY30</f>
         <v>0.37442270551683599</v>
       </c>
       <c r="AZ58" s="9">
-        <f t="shared" ref="AZ58:BM58" si="208">(AZ30-AZ33)/AZ30</f>
+        <f t="shared" ref="AZ58:BM58" si="211">(AZ30-AZ33)/AZ30</f>
         <v>0.41739926739926742</v>
       </c>
       <c r="BA58" s="9">
-        <f t="shared" si="208"/>
+        <f t="shared" si="211"/>
         <v>0.4999672938970412</v>
       </c>
       <c r="BB58" s="9">
-        <f t="shared" si="208"/>
+        <f t="shared" si="211"/>
         <v>0.55437146585471941</v>
       </c>
       <c r="BC58" s="9">
-        <f t="shared" si="208"/>
+        <f t="shared" si="211"/>
         <v>0.59904766985888447</v>
       </c>
       <c r="BD58" s="9">
-        <f t="shared" si="208"/>
+        <f t="shared" si="211"/>
         <v>0.64940111736450412</v>
       </c>
       <c r="BE58" s="9">
-        <f t="shared" si="208"/>
+        <f t="shared" si="211"/>
         <v>0.65280632159186858</v>
       </c>
       <c r="BF58" s="9">
-        <f t="shared" si="208"/>
+        <f t="shared" si="211"/>
         <v>0.67354771220519505</v>
       </c>
       <c r="BG58" s="9">
-        <f t="shared" si="208"/>
+        <f t="shared" si="211"/>
         <v>0.67373259624394921</v>
       </c>
       <c r="BH58" s="9">
-        <f t="shared" si="208"/>
+        <f t="shared" si="211"/>
         <v>0.65</v>
       </c>
       <c r="BI58" s="9">
-        <f t="shared" si="208"/>
+        <f t="shared" si="211"/>
         <v>0.65</v>
       </c>
       <c r="BJ58" s="9">
-        <f t="shared" si="208"/>
+        <f t="shared" si="211"/>
         <v>0.64999999999999991</v>
       </c>
       <c r="BK58" s="9">
-        <f t="shared" si="208"/>
+        <f t="shared" si="211"/>
         <v>0.65000000000000013</v>
       </c>
       <c r="BL58" s="9">
-        <f t="shared" si="208"/>
+        <f t="shared" si="211"/>
         <v>0.65000000000000013</v>
       </c>
       <c r="BM58" s="9">
-        <f t="shared" si="208"/>
+        <f t="shared" si="211"/>
         <v>0.64999999999999991</v>
       </c>
       <c r="BP58" s="1"/>
@@ -10632,151 +10658,151 @@
         <v>82</v>
       </c>
       <c r="G61" s="5">
-        <f t="shared" ref="G61:H61" si="209">+G62-G73</f>
+        <f t="shared" ref="G61:H61" si="212">+G62-G73</f>
         <v>77528</v>
       </c>
       <c r="H61" s="5">
-        <f t="shared" si="209"/>
+        <f t="shared" si="212"/>
         <v>75239</v>
       </c>
       <c r="I61" s="5">
-        <f t="shared" ref="I61:V61" si="210">+I62-I73</f>
+        <f t="shared" ref="I61:V61" si="213">+I62-I73</f>
         <v>72744</v>
       </c>
       <c r="J61" s="5">
-        <f t="shared" si="210"/>
+        <f t="shared" si="213"/>
         <v>78172</v>
       </c>
       <c r="K61" s="5">
-        <f t="shared" si="210"/>
+        <f t="shared" si="213"/>
         <v>83720</v>
       </c>
       <c r="L61" s="5">
-        <f t="shared" si="210"/>
+        <f t="shared" si="213"/>
         <v>79105</v>
       </c>
       <c r="M61" s="5">
-        <f t="shared" si="210"/>
+        <f t="shared" si="213"/>
         <v>61674</v>
       </c>
       <c r="N61" s="5">
-        <f t="shared" si="210"/>
+        <f t="shared" si="213"/>
         <v>61867</v>
       </c>
       <c r="O61" s="5">
-        <f t="shared" si="210"/>
+        <f t="shared" si="213"/>
         <v>65479</v>
       </c>
       <c r="P61" s="5">
-        <f t="shared" si="210"/>
+        <f t="shared" si="213"/>
         <v>58489</v>
       </c>
       <c r="Q61" s="5">
-        <f t="shared" si="210"/>
+        <f t="shared" si="213"/>
         <v>65632</v>
       </c>
       <c r="R61" s="5">
-        <f t="shared" si="210"/>
+        <f t="shared" si="213"/>
         <v>73904</v>
       </c>
       <c r="S61" s="5">
-        <f t="shared" si="210"/>
+        <f t="shared" si="213"/>
         <v>83872</v>
       </c>
       <c r="T61" s="5">
-        <f t="shared" si="210"/>
+        <f t="shared" si="213"/>
         <v>20165</v>
       </c>
       <c r="U61" s="5">
-        <f t="shared" si="210"/>
+        <f t="shared" si="213"/>
         <v>29386</v>
       </c>
       <c r="V61" s="5">
-        <f t="shared" si="210"/>
+        <f t="shared" si="213"/>
         <v>38513</v>
       </c>
       <c r="AC61" s="4">
-        <f t="shared" ref="AC61:AQ61" si="211">AC62</f>
+        <f t="shared" ref="AC61:AQ61" si="214">AC62</f>
         <v>3614</v>
       </c>
       <c r="AD61" s="4">
-        <f t="shared" si="211"/>
+        <f t="shared" si="214"/>
         <v>4750</v>
       </c>
       <c r="AE61" s="4">
-        <f t="shared" si="211"/>
+        <f t="shared" si="214"/>
         <v>6940</v>
       </c>
       <c r="AF61" s="4">
-        <f t="shared" si="211"/>
+        <f t="shared" si="214"/>
         <v>11312</v>
       </c>
       <c r="AG61" s="4">
-        <f t="shared" si="211"/>
+        <f t="shared" si="214"/>
         <v>18630</v>
       </c>
       <c r="AH61" s="4">
-        <f t="shared" si="211"/>
+        <f t="shared" si="214"/>
         <v>31608</v>
       </c>
       <c r="AI61" s="4">
-        <f t="shared" si="211"/>
+        <f t="shared" si="214"/>
         <v>41524</v>
       </c>
       <c r="AJ61" s="4">
-        <f t="shared" si="211"/>
+        <f t="shared" si="214"/>
         <v>45741</v>
       </c>
       <c r="AK61" s="4">
-        <f t="shared" si="211"/>
+        <f t="shared" si="214"/>
         <v>52843</v>
       </c>
       <c r="AL61" s="4">
-        <f t="shared" si="211"/>
+        <f t="shared" si="214"/>
         <v>62740</v>
       </c>
       <c r="AM61" s="4">
-        <f t="shared" si="211"/>
+        <f t="shared" si="214"/>
         <v>72802</v>
       </c>
       <c r="AN61" s="4">
-        <f t="shared" si="211"/>
+        <f t="shared" si="214"/>
         <v>48755</v>
       </c>
       <c r="AO61" s="4">
-        <f t="shared" si="211"/>
+        <f t="shared" si="214"/>
         <v>43393</v>
       </c>
       <c r="AP61" s="4">
-        <f t="shared" si="211"/>
+        <f t="shared" si="214"/>
         <v>33528</v>
       </c>
       <c r="AQ61" s="4">
-        <f t="shared" si="211"/>
+        <f t="shared" si="214"/>
         <v>30250</v>
       </c>
       <c r="AR61" s="4">
-        <f t="shared" ref="AR61:AW61" si="212">AR62-AR73</f>
+        <f t="shared" ref="AR61:AW61" si="215">AR62-AR73</f>
         <v>30634</v>
       </c>
       <c r="AS61" s="4">
-        <f t="shared" si="212"/>
+        <f t="shared" si="215"/>
         <v>38603</v>
       </c>
       <c r="AT61" s="4">
-        <f t="shared" si="212"/>
+        <f t="shared" si="215"/>
         <v>51716</v>
       </c>
       <c r="AU61" s="4">
-        <f t="shared" si="212"/>
+        <f t="shared" si="215"/>
         <v>60872</v>
       </c>
       <c r="AV61" s="4">
-        <f t="shared" si="212"/>
+        <f t="shared" si="215"/>
         <v>72266</v>
       </c>
       <c r="AW61" s="4">
-        <f t="shared" si="212"/>
+        <f t="shared" si="215"/>
         <v>77661</v>
       </c>
       <c r="BE61" s="5">
@@ -10784,35 +10810,35 @@
         <v>61867</v>
       </c>
       <c r="BF61" s="5">
-        <f t="shared" ref="BF61:BM61" si="213">+BE61+BF44</f>
+        <f t="shared" ref="BF61:BM61" si="216">+BE61+BF44</f>
         <v>137197.4</v>
       </c>
       <c r="BG61" s="5">
-        <f t="shared" si="213"/>
+        <f t="shared" si="216"/>
         <v>225654.26</v>
       </c>
       <c r="BH61" s="5">
-        <f t="shared" si="213"/>
+        <f t="shared" si="216"/>
         <v>324637.90996500006</v>
       </c>
       <c r="BI61" s="5">
-        <f t="shared" si="213"/>
+        <f t="shared" si="216"/>
         <v>435283.46279085259</v>
       </c>
       <c r="BJ61" s="5">
-        <f t="shared" si="213"/>
+        <f t="shared" si="216"/>
         <v>558805.51832430938</v>
       </c>
       <c r="BK61" s="5">
-        <f t="shared" si="213"/>
+        <f t="shared" si="216"/>
         <v>696541.55046272767</v>
       </c>
       <c r="BL61" s="5">
-        <f t="shared" si="213"/>
+        <f t="shared" si="216"/>
         <v>849964.23665623087</v>
       </c>
       <c r="BM61" s="5">
-        <f t="shared" si="213"/>
+        <f t="shared" si="216"/>
         <v>1020695.0216202373</v>
       </c>
     </row>
@@ -11903,151 +11929,151 @@
       <c r="E70" s="7"/>
       <c r="F70" s="7"/>
       <c r="G70" s="7">
-        <f t="shared" ref="G70:H70" si="214">SUM(G62:G69)</f>
+        <f t="shared" ref="G70:H70" si="217">SUM(G62:G69)</f>
         <v>301001</v>
       </c>
       <c r="H70" s="7">
-        <f t="shared" si="214"/>
+        <f t="shared" si="217"/>
         <v>304137</v>
       </c>
       <c r="I70" s="7">
-        <f t="shared" ref="I70:K70" si="215">SUM(I62:I69)</f>
+        <f t="shared" ref="I70:K70" si="218">SUM(I62:I69)</f>
         <v>308879</v>
       </c>
       <c r="J70" s="7">
-        <f t="shared" si="215"/>
+        <f t="shared" si="218"/>
         <v>333779</v>
       </c>
       <c r="K70" s="7">
-        <f t="shared" si="215"/>
+        <f t="shared" si="218"/>
         <v>335418</v>
       </c>
       <c r="L70" s="7">
-        <f t="shared" ref="L70" si="216">SUM(L62:L69)</f>
+        <f t="shared" ref="L70" si="219">SUM(L62:L69)</f>
         <v>340389</v>
       </c>
       <c r="M70" s="7">
-        <f t="shared" ref="M70:V70" si="217">SUM(M62:M69)</f>
+        <f t="shared" ref="M70:V70" si="220">SUM(M62:M69)</f>
         <v>344607</v>
       </c>
       <c r="N70" s="7">
-        <f t="shared" si="217"/>
+        <f t="shared" si="220"/>
         <v>364840</v>
       </c>
       <c r="O70" s="7">
-        <f t="shared" si="217"/>
+        <f t="shared" si="220"/>
         <v>359784</v>
       </c>
       <c r="P70" s="7">
-        <f t="shared" si="217"/>
+        <f t="shared" si="220"/>
         <v>364552</v>
       </c>
       <c r="Q70" s="7">
-        <f t="shared" si="217"/>
+        <f t="shared" si="220"/>
         <v>380088</v>
       </c>
       <c r="R70" s="7">
-        <f t="shared" si="217"/>
+        <f t="shared" si="220"/>
         <v>411976</v>
       </c>
       <c r="S70" s="7">
-        <f t="shared" si="217"/>
+        <f t="shared" si="220"/>
         <v>445785</v>
       </c>
       <c r="T70" s="7">
-        <f t="shared" si="217"/>
+        <f t="shared" si="220"/>
         <v>470558</v>
       </c>
       <c r="U70" s="7">
-        <f t="shared" si="217"/>
+        <f t="shared" si="220"/>
         <v>484275</v>
       </c>
       <c r="V70" s="7">
-        <f t="shared" si="217"/>
+        <f t="shared" si="220"/>
         <v>512163</v>
       </c>
       <c r="AC70" s="6">
-        <f t="shared" ref="AC70:AW70" si="218">SUM(AC62:AC69)</f>
+        <f t="shared" ref="AC70:AW70" si="221">SUM(AC62:AC69)</f>
         <v>5363</v>
       </c>
       <c r="AD70" s="6">
-        <f t="shared" si="218"/>
+        <f t="shared" si="221"/>
         <v>7210</v>
       </c>
       <c r="AE70" s="6">
-        <f t="shared" si="218"/>
+        <f t="shared" si="221"/>
         <v>10093</v>
       </c>
       <c r="AF70" s="6">
-        <f t="shared" si="218"/>
+        <f t="shared" si="221"/>
         <v>14387</v>
       </c>
       <c r="AG70" s="6">
-        <f t="shared" si="218"/>
+        <f t="shared" si="221"/>
         <v>22357</v>
       </c>
       <c r="AH70" s="6">
-        <f t="shared" si="218"/>
+        <f t="shared" si="221"/>
         <v>37156</v>
       </c>
       <c r="AI70" s="6">
-        <f t="shared" si="218"/>
+        <f t="shared" si="221"/>
         <v>52150</v>
       </c>
       <c r="AJ70" s="6">
-        <f t="shared" si="218"/>
+        <f t="shared" si="221"/>
         <v>59257</v>
       </c>
       <c r="AK70" s="6">
-        <f t="shared" si="218"/>
+        <f t="shared" si="221"/>
         <v>67646</v>
       </c>
       <c r="AL70" s="6">
-        <f t="shared" si="218"/>
+        <f t="shared" si="221"/>
         <v>79571</v>
       </c>
       <c r="AM70" s="6">
-        <f t="shared" si="218"/>
+        <f t="shared" si="221"/>
         <v>92389</v>
       </c>
       <c r="AN70" s="6">
-        <f t="shared" si="218"/>
+        <f t="shared" si="221"/>
         <v>70815</v>
       </c>
       <c r="AO70" s="6">
-        <f t="shared" si="218"/>
+        <f t="shared" si="221"/>
         <v>69597</v>
       </c>
       <c r="AP70" s="6">
-        <f t="shared" si="218"/>
+        <f t="shared" si="221"/>
         <v>63171</v>
       </c>
       <c r="AQ70" s="6">
-        <f t="shared" si="218"/>
+        <f t="shared" si="221"/>
         <v>72793</v>
       </c>
       <c r="AR70" s="6">
-        <f t="shared" si="218"/>
+        <f t="shared" si="221"/>
         <v>77888</v>
       </c>
       <c r="AS70" s="6">
-        <f t="shared" si="218"/>
+        <f t="shared" si="221"/>
         <v>86113</v>
       </c>
       <c r="AT70" s="6">
-        <f t="shared" si="218"/>
+        <f t="shared" si="221"/>
         <v>108704</v>
       </c>
       <c r="AU70" s="6">
-        <f t="shared" si="218"/>
+        <f t="shared" si="221"/>
         <v>121271</v>
       </c>
       <c r="AV70" s="6">
-        <f t="shared" si="218"/>
+        <f t="shared" si="221"/>
         <v>142431</v>
       </c>
       <c r="AW70" s="6">
-        <f t="shared" si="218"/>
+        <f t="shared" si="221"/>
         <v>172384</v>
       </c>
       <c r="BC70" s="7"/>
@@ -12109,6 +12135,12 @@
       </c>
       <c r="T72" s="4">
         <v>17695</v>
+      </c>
+      <c r="U72" s="4">
+        <v>18087</v>
+      </c>
+      <c r="V72" s="4">
+        <v>21996</v>
       </c>
       <c r="AC72" s="4">
         <v>324</v>
@@ -12374,6 +12406,12 @@
       <c r="T74" s="4">
         <v>8813</v>
       </c>
+      <c r="U74" s="4">
+        <v>10432</v>
+      </c>
+      <c r="V74" s="4">
+        <v>12564</v>
+      </c>
       <c r="AC74" s="4">
         <v>96</v>
       </c>
@@ -12506,6 +12544,14 @@
         <f>5787+2548+25890</f>
         <v>34225</v>
       </c>
+      <c r="U75" s="4">
+        <f>7311+26786+2469</f>
+        <v>36566</v>
+      </c>
+      <c r="V75" s="4">
+        <f>5017+27931+2618</f>
+        <v>35566</v>
+      </c>
       <c r="AC75" s="4">
         <v>305</v>
       </c>
@@ -12641,6 +12687,14 @@
         <f>2966+43068</f>
         <v>46034</v>
       </c>
+      <c r="U76" s="4">
+        <f>41888+2945</f>
+        <v>44833</v>
+      </c>
+      <c r="V76" s="4">
+        <f>57582+2602</f>
+        <v>60184</v>
+      </c>
       <c r="AC76" s="4">
         <v>0</v>
       </c>
@@ -12772,6 +12826,12 @@
       <c r="T77" s="4">
         <v>16362</v>
       </c>
+      <c r="U77" s="4">
+        <v>18023</v>
+      </c>
+      <c r="V77" s="4">
+        <v>19185</v>
+      </c>
       <c r="AC77" s="4">
         <v>188</v>
       </c>
@@ -12891,6 +12951,12 @@
       <c r="T78" s="4">
         <v>14155</v>
       </c>
+      <c r="U78" s="4">
+        <v>14469</v>
+      </c>
+      <c r="V78" s="4">
+        <v>15497</v>
+      </c>
       <c r="AC78" s="4">
         <v>0</v>
       </c>
@@ -13009,6 +13075,12 @@
       <c r="T79" s="4">
         <v>20787</v>
       </c>
+      <c r="U79" s="4">
+        <v>23271</v>
+      </c>
+      <c r="V79" s="4">
+        <v>27064</v>
+      </c>
       <c r="AC79" s="4">
         <v>0</v>
       </c>
@@ -13140,6 +13212,12 @@
       </c>
       <c r="T80" s="4">
         <v>238268</v>
+      </c>
+      <c r="U80" s="4">
+        <v>253152</v>
+      </c>
+      <c r="V80" s="4">
+        <v>268477</v>
       </c>
       <c r="AC80" s="4">
         <v>4450</v>
@@ -13223,141 +13301,147 @@
         <v>301001</v>
       </c>
       <c r="H81" s="7">
-        <f t="shared" ref="H81" si="219">SUM(H72:H80)</f>
+        <f t="shared" ref="H81" si="222">SUM(H72:H80)</f>
         <v>304137</v>
       </c>
       <c r="I81" s="7">
-        <f t="shared" ref="I81:L81" si="220">SUM(I72:I80)</f>
+        <f t="shared" ref="I81:L81" si="223">SUM(I72:I80)</f>
         <v>308879</v>
       </c>
       <c r="J81" s="7">
-        <f t="shared" si="220"/>
+        <f t="shared" si="223"/>
         <v>333779</v>
       </c>
       <c r="K81" s="7">
-        <f t="shared" si="220"/>
+        <f t="shared" si="223"/>
         <v>335418</v>
       </c>
       <c r="L81" s="7">
-        <f t="shared" si="220"/>
+        <f t="shared" si="223"/>
         <v>340389</v>
       </c>
       <c r="M81" s="7">
-        <f t="shared" ref="M81:S81" si="221">SUM(M72:M80)</f>
+        <f t="shared" ref="M81:S81" si="224">SUM(M72:M80)</f>
         <v>344607</v>
       </c>
       <c r="N81" s="7">
-        <f t="shared" si="221"/>
+        <f t="shared" si="224"/>
         <v>364840</v>
       </c>
       <c r="O81" s="7">
-        <f t="shared" si="221"/>
+        <f t="shared" si="224"/>
         <v>359784</v>
       </c>
       <c r="P81" s="7">
-        <f t="shared" si="221"/>
+        <f t="shared" si="224"/>
         <v>364552</v>
       </c>
       <c r="Q81" s="7">
-        <f t="shared" si="221"/>
+        <f t="shared" si="224"/>
         <v>380088</v>
       </c>
       <c r="R81" s="7">
-        <f t="shared" si="221"/>
+        <f t="shared" si="224"/>
         <v>411976</v>
       </c>
       <c r="S81" s="7">
-        <f t="shared" si="221"/>
+        <f t="shared" si="224"/>
         <v>445785</v>
       </c>
       <c r="T81" s="7">
-        <f t="shared" ref="T81" si="222">SUM(T72:T80)</f>
+        <f t="shared" ref="T81:V81" si="225">SUM(T72:T80)</f>
         <v>470558</v>
       </c>
-      <c r="U81" s="7"/>
-      <c r="V81" s="7"/>
+      <c r="U81" s="7">
+        <f t="shared" si="225"/>
+        <v>484275</v>
+      </c>
+      <c r="V81" s="7">
+        <f t="shared" si="225"/>
+        <v>512163</v>
+      </c>
       <c r="AC81" s="6">
-        <f t="shared" ref="AC81:AW81" si="223">SUM(AC72:AC80)</f>
+        <f t="shared" ref="AC81:AW81" si="226">SUM(AC72:AC80)</f>
         <v>5363</v>
       </c>
       <c r="AD81" s="6">
-        <f t="shared" si="223"/>
+        <f t="shared" si="226"/>
         <v>7210</v>
       </c>
       <c r="AE81" s="6">
-        <f t="shared" si="223"/>
+        <f t="shared" si="226"/>
         <v>10093</v>
       </c>
       <c r="AF81" s="6">
-        <f t="shared" si="223"/>
+        <f t="shared" si="226"/>
         <v>14387</v>
       </c>
       <c r="AG81" s="6">
-        <f t="shared" si="223"/>
+        <f t="shared" si="226"/>
         <v>22357</v>
       </c>
       <c r="AH81" s="6">
-        <f t="shared" si="223"/>
+        <f t="shared" si="226"/>
         <v>37156</v>
       </c>
       <c r="AI81" s="6">
-        <f t="shared" si="223"/>
+        <f t="shared" si="226"/>
         <v>52150</v>
       </c>
       <c r="AJ81" s="6">
-        <f t="shared" si="223"/>
+        <f t="shared" si="226"/>
         <v>59257</v>
       </c>
       <c r="AK81" s="6">
-        <f t="shared" si="223"/>
+        <f t="shared" si="226"/>
         <v>67646</v>
       </c>
       <c r="AL81" s="6">
-        <f t="shared" si="223"/>
+        <f t="shared" si="226"/>
         <v>79571</v>
       </c>
       <c r="AM81" s="6">
-        <f t="shared" si="223"/>
+        <f t="shared" si="226"/>
         <v>92389</v>
       </c>
       <c r="AN81" s="6">
-        <f t="shared" si="223"/>
+        <f t="shared" si="226"/>
         <v>70815</v>
       </c>
       <c r="AO81" s="6">
-        <f t="shared" si="223"/>
+        <f t="shared" si="226"/>
         <v>69597</v>
       </c>
       <c r="AP81" s="6">
-        <f t="shared" si="223"/>
+        <f t="shared" si="226"/>
         <v>63171</v>
       </c>
       <c r="AQ81" s="6">
-        <f t="shared" si="223"/>
+        <f t="shared" si="226"/>
         <v>72793</v>
       </c>
       <c r="AR81" s="6">
-        <f t="shared" si="223"/>
+        <f t="shared" si="226"/>
         <v>77888</v>
       </c>
       <c r="AS81" s="6">
-        <f t="shared" si="223"/>
+        <f t="shared" si="226"/>
         <v>86113</v>
       </c>
       <c r="AT81" s="6">
-        <f t="shared" si="223"/>
+        <f t="shared" si="226"/>
         <v>108704</v>
       </c>
       <c r="AU81" s="6">
-        <f t="shared" si="223"/>
+        <f t="shared" si="226"/>
         <v>121271</v>
       </c>
       <c r="AV81" s="6">
-        <f t="shared" si="223"/>
+        <f t="shared" si="226"/>
         <v>142431</v>
       </c>
       <c r="AW81" s="6">
-        <f t="shared" si="223"/>
+        <f t="shared" si="226"/>
         <v>172384</v>
       </c>
       <c r="BC81" s="7"/>
@@ -13374,67 +13458,67 @@
       <c r="E83" s="5"/>
       <c r="F83" s="5"/>
       <c r="G83" s="5">
-        <f t="shared" ref="G83:H83" si="224">G44</f>
+        <f t="shared" ref="G83:H83" si="227">G44</f>
         <v>13893</v>
       </c>
       <c r="H83" s="5">
-        <f t="shared" si="224"/>
+        <f t="shared" si="227"/>
         <v>15463</v>
       </c>
       <c r="I83" s="5">
-        <f t="shared" ref="I83:V83" si="225">I44</f>
+        <f t="shared" ref="I83:V84" si="228">I44</f>
         <v>15457</v>
       </c>
       <c r="J83" s="5">
-        <f t="shared" si="225"/>
+        <f t="shared" si="228"/>
         <v>16458</v>
       </c>
       <c r="K83" s="5">
-        <f t="shared" si="225"/>
+        <f t="shared" si="228"/>
         <v>20505</v>
       </c>
       <c r="L83" s="5">
-        <f t="shared" si="225"/>
+        <f t="shared" si="228"/>
         <v>18765</v>
       </c>
       <c r="M83" s="5">
-        <f t="shared" si="225"/>
+        <f t="shared" si="228"/>
         <v>16728</v>
       </c>
       <c r="N83" s="5">
-        <f t="shared" si="225"/>
+        <f t="shared" si="228"/>
         <v>16740</v>
       </c>
       <c r="O83" s="5">
-        <f t="shared" si="225"/>
+        <f t="shared" si="228"/>
         <v>17556</v>
       </c>
       <c r="P83" s="5">
-        <f t="shared" si="225"/>
+        <f t="shared" si="228"/>
         <v>16425</v>
       </c>
       <c r="Q83" s="5">
-        <f t="shared" si="225"/>
+        <f t="shared" si="228"/>
         <v>18299</v>
       </c>
       <c r="R83" s="5">
-        <f t="shared" si="225"/>
+        <f t="shared" si="228"/>
         <v>20081</v>
       </c>
       <c r="S83" s="5">
-        <f t="shared" si="225"/>
+        <f t="shared" si="228"/>
         <v>22291</v>
       </c>
       <c r="T83" s="5">
-        <f t="shared" si="225"/>
+        <f t="shared" si="228"/>
         <v>21870</v>
       </c>
       <c r="U83" s="5">
-        <f t="shared" si="225"/>
+        <f t="shared" si="228"/>
         <v>21660</v>
       </c>
       <c r="V83" s="5">
-        <f t="shared" si="225"/>
+        <f t="shared" si="228"/>
         <v>22036</v>
       </c>
       <c r="BC83" s="5"/>
@@ -13492,6 +13576,12 @@
       <c r="T84" s="4">
         <v>21870</v>
       </c>
+      <c r="U84" s="4">
+        <v>21660</v>
+      </c>
+      <c r="V84" s="4">
+        <v>22036</v>
+      </c>
       <c r="BC84" s="5"/>
       <c r="BD84" s="5"/>
       <c r="BE84" s="5"/>
@@ -13547,6 +13637,12 @@
       <c r="T85" s="4">
         <v>5959</v>
       </c>
+      <c r="U85" s="4">
+        <v>6027</v>
+      </c>
+      <c r="V85" s="4">
+        <v>6380</v>
+      </c>
       <c r="BC85" s="5"/>
       <c r="BD85" s="5"/>
       <c r="BE85" s="5"/>
@@ -13602,6 +13698,12 @@
       <c r="T86" s="4">
         <v>2828</v>
       </c>
+      <c r="U86" s="4">
+        <v>2703</v>
+      </c>
+      <c r="V86" s="4">
+        <v>2696</v>
+      </c>
       <c r="BC86" s="5"/>
       <c r="BD86" s="5"/>
       <c r="BE86" s="5"/>
@@ -13657,6 +13759,12 @@
       <c r="T87" s="4">
         <v>198</v>
       </c>
+      <c r="U87" s="4">
+        <v>49</v>
+      </c>
+      <c r="V87" s="4">
+        <v>44</v>
+      </c>
       <c r="BC87" s="5"/>
       <c r="BD87" s="5"/>
       <c r="BE87" s="5"/>
@@ -13711,6 +13819,12 @@
       </c>
       <c r="T88" s="4">
         <v>-1702</v>
+      </c>
+      <c r="U88" s="4">
+        <v>-1323</v>
+      </c>
+      <c r="V88" s="4">
+        <v>-1145</v>
       </c>
       <c r="BC88" s="5"/>
       <c r="BD88" s="5"/>
@@ -13781,6 +13895,14 @@
         <f>-2951+1474+725-1427-2521-5538-1554+1518-26</f>
         <v>-10300</v>
       </c>
+      <c r="U89" s="4">
+        <f>-1408+106+1152-554-407-181+1414+1715+6</f>
+        <v>1843</v>
+      </c>
+      <c r="V89" s="4">
+        <f>-13246+55-2528-1240+4204+15657-806+4652+436</f>
+        <v>7184</v>
+      </c>
       <c r="BC89" s="5"/>
       <c r="BD89" s="5"/>
       <c r="BE89" s="5"/>
@@ -13795,47 +13917,47 @@
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
       <c r="G90" s="5">
-        <f t="shared" ref="G90:H90" si="226">SUM(G84:G89)</f>
+        <f t="shared" ref="G90:H90" si="229">SUM(G84:G89)</f>
         <v>19335</v>
       </c>
       <c r="H90" s="5">
-        <f t="shared" si="226"/>
+        <f t="shared" si="229"/>
         <v>12516</v>
       </c>
       <c r="I90" s="5">
-        <f t="shared" ref="I90:K90" si="227">SUM(I84:I89)</f>
+        <f t="shared" ref="I90:K90" si="230">SUM(I84:I89)</f>
         <v>22179</v>
       </c>
       <c r="J90" s="5">
-        <f t="shared" si="227"/>
+        <f t="shared" si="230"/>
         <v>22710</v>
       </c>
       <c r="K90" s="5">
-        <f t="shared" si="227"/>
+        <f t="shared" si="230"/>
         <v>24540</v>
       </c>
       <c r="L90" s="5">
-        <f t="shared" ref="L90" si="228">SUM(L84:L89)</f>
+        <f t="shared" ref="L90" si="231">SUM(L84:L89)</f>
         <v>14480</v>
       </c>
       <c r="M90" s="5">
-        <f t="shared" ref="M90:Q90" si="229">SUM(M84:M89)</f>
+        <f t="shared" ref="M90:Q90" si="232">SUM(M84:M89)</f>
         <v>25386</v>
       </c>
       <c r="N90" s="5">
-        <f t="shared" si="229"/>
+        <f t="shared" si="232"/>
         <v>24629</v>
       </c>
       <c r="O90" s="5">
-        <f t="shared" si="229"/>
+        <f t="shared" si="232"/>
         <v>23198</v>
       </c>
       <c r="P90" s="5">
-        <f t="shared" si="229"/>
+        <f t="shared" si="232"/>
         <v>11173</v>
       </c>
       <c r="Q90" s="5">
-        <f t="shared" si="229"/>
+        <f t="shared" si="232"/>
         <v>24441</v>
       </c>
       <c r="R90" s="5">
@@ -13850,8 +13972,14 @@
         <f>SUM(T84:T89)</f>
         <v>18853</v>
       </c>
-      <c r="U90" s="5"/>
-      <c r="V90" s="5"/>
+      <c r="U90" s="5">
+        <f t="shared" ref="U90:V90" si="233">SUM(U84:U89)</f>
+        <v>30959</v>
+      </c>
+      <c r="V90" s="5">
+        <f t="shared" si="233"/>
+        <v>37195</v>
+      </c>
       <c r="BC90" s="5"/>
       <c r="BD90" s="5"/>
       <c r="BE90" s="5"/>
@@ -13925,6 +14053,12 @@
       <c r="T92" s="4">
         <v>-9735</v>
       </c>
+      <c r="U92" s="4">
+        <v>-10952</v>
+      </c>
+      <c r="V92" s="4">
+        <v>-13873</v>
+      </c>
       <c r="BC92" s="5"/>
       <c r="BD92" s="5"/>
       <c r="BE92" s="5"/>
@@ -13979,6 +14113,12 @@
       </c>
       <c r="T93" s="4">
         <v>-65029</v>
+      </c>
+      <c r="U93" s="4">
+        <v>-1575</v>
+      </c>
+      <c r="V93" s="4">
+        <v>-1342</v>
       </c>
       <c r="BC93" s="5"/>
       <c r="BD93" s="5"/>
@@ -14049,6 +14189,14 @@
         <f>-4258+4150+1600</f>
         <v>1492</v>
       </c>
+      <c r="U94" s="4">
+        <f>-2183+3350+1941</f>
+        <v>3108</v>
+      </c>
+      <c r="V94" s="4">
+        <f>-2831+1557+2023</f>
+        <v>749</v>
+      </c>
       <c r="BC94" s="5"/>
       <c r="BD94" s="5"/>
       <c r="BE94" s="5"/>
@@ -14104,6 +14252,12 @@
       <c r="T95" s="4">
         <v>1347</v>
       </c>
+      <c r="U95" s="4">
+        <v>-1281</v>
+      </c>
+      <c r="V95" s="4">
+        <v>-382</v>
+      </c>
       <c r="BC95" s="5"/>
       <c r="BD95" s="5"/>
       <c r="BE95" s="5"/>
@@ -14118,60 +14272,68 @@
       <c r="E96" s="5"/>
       <c r="F96" s="5"/>
       <c r="G96" s="5">
-        <f t="shared" ref="G96:H96" si="230">SUM(G92:G95)</f>
+        <f t="shared" ref="G96:H96" si="234">SUM(G92:G95)</f>
         <v>-5371</v>
       </c>
       <c r="H96" s="5">
-        <f t="shared" si="230"/>
+        <f t="shared" si="234"/>
         <v>-1669</v>
       </c>
       <c r="I96" s="5">
-        <f t="shared" ref="I96:L96" si="231">SUM(I92:I95)</f>
+        <f t="shared" ref="I96:L96" si="235">SUM(I92:I95)</f>
         <v>-9684</v>
       </c>
       <c r="J96" s="5">
-        <f t="shared" si="231"/>
+        <f t="shared" si="235"/>
         <v>-10853</v>
       </c>
       <c r="K96" s="5">
-        <f t="shared" si="231"/>
+        <f t="shared" si="235"/>
         <v>-3250</v>
       </c>
       <c r="L96" s="5">
-        <f t="shared" si="231"/>
+        <f t="shared" si="235"/>
         <v>-1161</v>
       </c>
       <c r="M96" s="5">
-        <f t="shared" ref="M96:T96" si="232">SUM(M92:M95)</f>
+        <f t="shared" ref="M96:V96" si="236">SUM(M92:M95)</f>
         <v>-16171</v>
       </c>
       <c r="N96" s="5">
-        <f t="shared" si="232"/>
+        <f t="shared" si="236"/>
         <v>-9729</v>
       </c>
       <c r="O96" s="5">
-        <f t="shared" si="232"/>
+        <f t="shared" si="236"/>
         <v>-3132</v>
       </c>
       <c r="P96" s="5">
-        <f t="shared" si="232"/>
+        <f t="shared" si="236"/>
         <v>-7150</v>
       </c>
       <c r="Q96" s="5">
-        <f t="shared" si="232"/>
+        <f t="shared" si="236"/>
         <v>-3264</v>
       </c>
       <c r="R96" s="5">
-        <f t="shared" si="232"/>
+        <f t="shared" si="236"/>
         <v>-9134</v>
       </c>
       <c r="S96" s="5">
-        <f t="shared" si="232"/>
+        <f t="shared" si="236"/>
         <v>503</v>
       </c>
       <c r="T96" s="5">
-        <f t="shared" si="232"/>
+        <f t="shared" si="236"/>
         <v>-71925</v>
+      </c>
+      <c r="U96" s="5">
+        <f t="shared" si="236"/>
+        <v>-10700</v>
+      </c>
+      <c r="V96" s="5">
+        <f t="shared" si="236"/>
+        <v>-14848</v>
       </c>
       <c r="BC96" s="5"/>
       <c r="BD96" s="5"/>
@@ -14478,23 +14640,23 @@
       <c r="E103" s="5"/>
       <c r="F103" s="5"/>
       <c r="G103" s="5">
-        <f t="shared" ref="G103:H103" si="233">SUM(G98:G102)</f>
+        <f t="shared" ref="G103:H103" si="237">SUM(G98:G102)</f>
         <v>-10289</v>
       </c>
       <c r="H103" s="5">
-        <f t="shared" si="233"/>
+        <f t="shared" si="237"/>
         <v>-13634</v>
       </c>
       <c r="I103" s="5">
-        <f t="shared" ref="I103:K103" si="234">SUM(I98:I102)</f>
+        <f t="shared" ref="I103:K103" si="238">SUM(I98:I102)</f>
         <v>-13192</v>
       </c>
       <c r="J103" s="5">
-        <f t="shared" si="234"/>
+        <f t="shared" si="238"/>
         <v>-11371</v>
       </c>
       <c r="K103" s="5">
-        <f t="shared" si="234"/>
+        <f t="shared" si="238"/>
         <v>-16276</v>
       </c>
       <c r="L103" s="5">
@@ -14518,19 +14680,19 @@
         <v>-11349</v>
       </c>
       <c r="Q103" s="5">
-        <f t="shared" ref="Q103:T103" si="235">SUM(Q98:Q102)</f>
+        <f t="shared" ref="Q103:T103" si="239">SUM(Q98:Q102)</f>
         <v>-10290</v>
       </c>
       <c r="R103" s="5">
-        <f t="shared" si="235"/>
+        <f t="shared" si="239"/>
         <v>-11413</v>
       </c>
       <c r="S103" s="5">
-        <f t="shared" si="235"/>
+        <f t="shared" si="239"/>
         <v>14761</v>
       </c>
       <c r="T103" s="5">
-        <f t="shared" si="235"/>
+        <f t="shared" si="239"/>
         <v>-10147</v>
       </c>
       <c r="BC103" s="5"/>
@@ -14590,23 +14752,23 @@
         <v>67</v>
       </c>
       <c r="G105" s="5">
-        <f t="shared" ref="G105:H105" si="236">G103+G104+G96+G90</f>
+        <f t="shared" ref="G105:H105" si="240">G103+G104+G96+G90</f>
         <v>3629</v>
       </c>
       <c r="H105" s="5">
-        <f t="shared" si="236"/>
+        <f t="shared" si="240"/>
         <v>-2773</v>
       </c>
       <c r="I105" s="5">
-        <f t="shared" ref="I105:K105" si="237">I103+I104+I96+I90</f>
+        <f t="shared" ref="I105:K105" si="241">I103+I104+I96+I90</f>
         <v>-730</v>
       </c>
       <c r="J105" s="5">
-        <f t="shared" si="237"/>
+        <f t="shared" si="241"/>
         <v>522</v>
       </c>
       <c r="K105" s="5">
-        <f t="shared" si="237"/>
+        <f t="shared" si="241"/>
         <v>4941</v>
       </c>
       <c r="L105" s="5">
@@ -14630,19 +14792,19 @@
         <v>-7238</v>
       </c>
       <c r="Q105" s="5">
-        <f t="shared" ref="Q105:T105" si="238">Q103+Q104+Q96+Q90</f>
+        <f t="shared" ref="Q105:T105" si="242">Q103+Q104+Q96+Q90</f>
         <v>10916</v>
       </c>
       <c r="R105" s="5">
-        <f t="shared" si="238"/>
+        <f t="shared" si="242"/>
         <v>8142</v>
       </c>
       <c r="S105" s="5">
-        <f t="shared" si="238"/>
+        <f t="shared" si="242"/>
         <v>45748</v>
       </c>
       <c r="T105" s="5">
-        <f t="shared" si="238"/>
+        <f t="shared" si="242"/>
         <v>-63147</v>
       </c>
     </row>
@@ -14651,23 +14813,23 @@
         <v>72</v>
       </c>
       <c r="G107" s="5">
-        <f t="shared" ref="G107:K107" si="239">G90+G92</f>
+        <f t="shared" ref="G107:K107" si="243">G90+G92</f>
         <v>14428</v>
       </c>
       <c r="H107" s="5">
-        <f t="shared" si="239"/>
+        <f t="shared" si="243"/>
         <v>8342</v>
       </c>
       <c r="I107" s="5">
-        <f t="shared" si="239"/>
+        <f t="shared" si="243"/>
         <v>17090</v>
       </c>
       <c r="J107" s="5">
-        <f t="shared" si="239"/>
+        <f t="shared" si="243"/>
         <v>16258</v>
       </c>
       <c r="K107" s="5">
-        <f t="shared" si="239"/>
+        <f t="shared" si="243"/>
         <v>18730</v>
       </c>
       <c r="L107" s="5">
@@ -14675,11 +14837,11 @@
         <v>8615</v>
       </c>
       <c r="M107" s="5">
-        <f t="shared" ref="M107:N107" si="240">M90+M92</f>
+        <f t="shared" ref="M107:N107" si="244">M90+M92</f>
         <v>20046</v>
       </c>
       <c r="N107" s="5">
-        <f t="shared" si="240"/>
+        <f t="shared" si="244"/>
         <v>17758</v>
       </c>
       <c r="O107" s="5">
@@ -14691,19 +14853,19 @@
         <v>4899</v>
       </c>
       <c r="Q107" s="5">
-        <f t="shared" ref="Q107:T107" si="241">Q90+Q92</f>
+        <f t="shared" ref="Q107:T107" si="245">Q90+Q92</f>
         <v>17834</v>
       </c>
       <c r="R107" s="5">
-        <f t="shared" si="241"/>
+        <f t="shared" si="245"/>
         <v>19827</v>
       </c>
       <c r="S107" s="5">
-        <f t="shared" si="241"/>
+        <f t="shared" si="245"/>
         <v>20666</v>
       </c>
       <c r="T107" s="5">
-        <f t="shared" si="241"/>
+        <f t="shared" si="245"/>
         <v>9118</v>
       </c>
     </row>
@@ -14712,43 +14874,43 @@
         <v>103</v>
       </c>
       <c r="K108" s="4">
-        <f t="shared" ref="K108:P108" si="242">SUM(H107:K107)</f>
+        <f t="shared" ref="K108:P108" si="246">SUM(H107:K107)</f>
         <v>60420</v>
       </c>
       <c r="L108" s="4">
-        <f t="shared" si="242"/>
+        <f t="shared" si="246"/>
         <v>60693</v>
       </c>
       <c r="M108" s="4">
-        <f t="shared" si="242"/>
+        <f t="shared" si="246"/>
         <v>63649</v>
       </c>
       <c r="N108" s="4">
-        <f t="shared" si="242"/>
+        <f t="shared" si="246"/>
         <v>65149</v>
       </c>
       <c r="O108" s="4">
-        <f t="shared" si="242"/>
+        <f t="shared" si="246"/>
         <v>63334</v>
       </c>
       <c r="P108" s="4">
-        <f t="shared" si="242"/>
+        <f t="shared" si="246"/>
         <v>59618</v>
       </c>
       <c r="Q108" s="4">
-        <f t="shared" ref="Q108:T108" si="243">SUM(N107:Q107)</f>
+        <f t="shared" ref="Q108:T108" si="247">SUM(N107:Q107)</f>
         <v>57406</v>
       </c>
       <c r="R108" s="4">
-        <f t="shared" si="243"/>
+        <f t="shared" si="247"/>
         <v>59475</v>
       </c>
       <c r="S108" s="4">
-        <f t="shared" si="243"/>
+        <f t="shared" si="247"/>
         <v>63226</v>
       </c>
       <c r="T108" s="4">
-        <f t="shared" si="243"/>
+        <f t="shared" si="247"/>
         <v>67445</v>
       </c>
     </row>
@@ -14757,27 +14919,27 @@
         <v>465</v>
       </c>
       <c r="O109" s="12">
-        <f t="shared" ref="O109:T109" si="244">+O108/K108-1</f>
+        <f t="shared" ref="O109:T109" si="248">+O108/K108-1</f>
         <v>4.8229063224098034E-2</v>
       </c>
       <c r="P109" s="12">
-        <f t="shared" si="244"/>
+        <f t="shared" si="248"/>
         <v>-1.7712092004020241E-2</v>
       </c>
       <c r="Q109" s="12">
-        <f t="shared" si="244"/>
+        <f t="shared" si="248"/>
         <v>-9.8084808873666551E-2</v>
       </c>
       <c r="R109" s="12">
-        <f t="shared" si="244"/>
+        <f t="shared" si="248"/>
         <v>-8.7092664507513518E-2</v>
       </c>
       <c r="S109" s="12">
-        <f t="shared" si="244"/>
+        <f t="shared" si="248"/>
         <v>-1.7052452079451275E-3</v>
       </c>
       <c r="T109" s="12">
-        <f t="shared" si="244"/>
+        <f t="shared" si="248"/>
         <v>0.13128585326579212</v>
       </c>
     </row>
@@ -14786,39 +14948,39 @@
         <v>466</v>
       </c>
       <c r="K110" s="4">
-        <f t="shared" ref="K110:S110" si="245">SUM(H92:K92)</f>
+        <f t="shared" ref="K110:S110" si="249">SUM(H92:K92)</f>
         <v>-21525</v>
       </c>
       <c r="L110" s="4">
-        <f t="shared" si="245"/>
+        <f t="shared" si="249"/>
         <v>-23216</v>
       </c>
       <c r="M110" s="4">
-        <f t="shared" si="245"/>
+        <f t="shared" si="249"/>
         <v>-23467</v>
       </c>
       <c r="N110" s="4">
-        <f t="shared" si="245"/>
+        <f t="shared" si="249"/>
         <v>-23886</v>
       </c>
       <c r="O110" s="4">
-        <f t="shared" si="245"/>
+        <f t="shared" si="249"/>
         <v>-24359</v>
       </c>
       <c r="P110" s="4">
-        <f t="shared" si="245"/>
+        <f t="shared" si="249"/>
         <v>-24768</v>
       </c>
       <c r="Q110" s="4">
-        <f t="shared" si="245"/>
+        <f t="shared" si="249"/>
         <v>-26035</v>
       </c>
       <c r="R110" s="4">
-        <f t="shared" si="245"/>
+        <f t="shared" si="249"/>
         <v>-28107</v>
       </c>
       <c r="S110" s="4">
-        <f t="shared" si="245"/>
+        <f t="shared" si="249"/>
         <v>-31741</v>
       </c>
       <c r="T110" s="4">
@@ -14831,23 +14993,23 @@
         <v>465</v>
       </c>
       <c r="O111" s="12">
-        <f t="shared" ref="O111:S111" si="246">+O110/K110-1</f>
+        <f t="shared" ref="O111:S111" si="250">+O110/K110-1</f>
         <v>0.13166085946573758</v>
       </c>
       <c r="P111" s="12">
-        <f t="shared" si="246"/>
+        <f t="shared" si="250"/>
         <v>6.6850447966919413E-2</v>
       </c>
       <c r="Q111" s="12">
-        <f t="shared" si="246"/>
+        <f t="shared" si="250"/>
         <v>0.10943026377466225</v>
       </c>
       <c r="R111" s="12">
-        <f t="shared" si="246"/>
+        <f t="shared" si="250"/>
         <v>0.17671439336850048</v>
       </c>
       <c r="S111" s="12">
-        <f t="shared" si="246"/>
+        <f t="shared" si="250"/>
         <v>0.3030502073155712</v>
       </c>
       <c r="T111" s="12">
@@ -15055,95 +15217,95 @@
         <v>2</v>
       </c>
       <c r="AC117" s="4">
-        <f t="shared" ref="AC117:AY117" si="247">AC116*AC46</f>
+        <f t="shared" ref="AC117:AY117" si="251">AC116*AC46</f>
         <v>20734.741379310344</v>
       </c>
       <c r="AD117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>36544.838709677417</v>
       </c>
       <c r="AE117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>49327.24832214765</v>
       </c>
       <c r="AF117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>114885.89743906935</v>
       </c>
       <c r="AG117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>184709.73040305718</v>
       </c>
       <c r="AH117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>372704.58101536665</v>
       </c>
       <c r="AI117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>298261.112605042</v>
       </c>
       <c r="AJ117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>266298.08220699872</v>
       </c>
       <c r="AK117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>222567.08981033842</v>
       </c>
       <c r="AL117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>236906.16184222695</v>
       </c>
       <c r="AM117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>252642.2008830022</v>
       </c>
       <c r="AN117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>260731.99813293503</v>
       </c>
       <c r="AO117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>247113.52251981141</v>
       </c>
       <c r="AP117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>265170.46442666667</v>
       </c>
       <c r="AQ117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>298326.78203723987</v>
       </c>
       <c r="AR117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>151214.58181818182</v>
       </c>
       <c r="AS117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>242693.07615855773</v>
       </c>
       <c r="AT117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>213717.28455478634</v>
       </c>
       <c r="AU117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>198199.0335202195</v>
       </c>
       <c r="AV117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>206380.61592027853</v>
       </c>
       <c r="AW117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>290064.69972083991</v>
       </c>
       <c r="AX117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>377052.05051894463</v>
       </c>
       <c r="AY117" s="4">
-        <f t="shared" si="247"/>
+        <f t="shared" si="251"/>
         <v>436539.84856262838</v>
       </c>
     </row>
@@ -15152,95 +15314,95 @@
         <v>5</v>
       </c>
       <c r="AC118" s="4">
-        <f t="shared" ref="AC118:AY118" si="248">AC117-AC61</f>
+        <f t="shared" ref="AC118:AY118" si="252">AC117-AC61</f>
         <v>17120.741379310344</v>
       </c>
       <c r="AD118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>31794.838709677417</v>
       </c>
       <c r="AE118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>42387.24832214765</v>
       </c>
       <c r="AF118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>103573.89743906935</v>
       </c>
       <c r="AG118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>166079.73040305718</v>
       </c>
       <c r="AH118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>341096.58101536665</v>
       </c>
       <c r="AI118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>256737.112605042</v>
       </c>
       <c r="AJ118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>220557.08220699872</v>
       </c>
       <c r="AK118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>169724.08981033842</v>
       </c>
       <c r="AL118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>174166.16184222695</v>
       </c>
       <c r="AM118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>179840.2008830022</v>
       </c>
       <c r="AN118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>211976.99813293503</v>
       </c>
       <c r="AO118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>203720.52251981141</v>
       </c>
       <c r="AP118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>231642.46442666667</v>
       </c>
       <c r="AQ118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>268076.78203723987</v>
       </c>
       <c r="AR118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>120580.58181818182</v>
       </c>
       <c r="AS118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>204090.07615855773</v>
       </c>
       <c r="AT118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>162001.28455478634</v>
       </c>
       <c r="AU118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>137327.0335202195</v>
       </c>
       <c r="AV118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>134114.61592027853</v>
       </c>
       <c r="AW118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>212403.69972083991</v>
       </c>
       <c r="AX118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>377052.05051894463</v>
       </c>
       <c r="AY118" s="4">
-        <f t="shared" si="248"/>
+        <f t="shared" si="252"/>
         <v>436539.84856262838</v>
       </c>
     </row>
@@ -15249,95 +15411,95 @@
         <v>223</v>
       </c>
       <c r="AC119" s="24">
-        <f t="shared" ref="AC119:AY119" si="249">AC118/AC44</f>
+        <f t="shared" ref="AC119:AY119" si="253">AC118/AC44</f>
         <v>13.85173250753264</v>
       </c>
       <c r="AD119" s="24">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>21.21069960618907</v>
       </c>
       <c r="AE119" s="24">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>19.310819281160661</v>
       </c>
       <c r="AF119" s="24">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>29.986652414322336</v>
       </c>
       <c r="AG119" s="24">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>34.905365784585371</v>
       </c>
       <c r="AH119" s="24">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>44.733977838080875</v>
       </c>
       <c r="AI119" s="24">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>27.710427696172907</v>
       </c>
       <c r="AJ119" s="24">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>27.989477437436385</v>
       </c>
       <c r="AK119" s="24">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>21.427103877078451</v>
       </c>
       <c r="AL119" s="24">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>17.311018968514755</v>
       </c>
       <c r="AM119" s="24">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>21.950470021115855</v>
       </c>
       <c r="AN119" s="24">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>17.298596224329607</v>
       </c>
       <c r="AO119" s="24">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>16.16957873798011</v>
       </c>
       <c r="AP119" s="24">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>16.469425128095747</v>
       </c>
       <c r="AQ119" s="24">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>15.161856345073236</v>
       </c>
       <c r="AR119" s="25">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>8.0931996656273455</v>
       </c>
       <c r="AS119" s="25">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>10.844894848746359</v>
       </c>
       <c r="AT119" s="25">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>6.9978956611138807</v>
       </c>
       <c r="AU119" s="25">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>5.9266770325069915</v>
       </c>
       <c r="AV119" s="25">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>6.1343189827689946</v>
       </c>
       <c r="AW119" s="25">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>9.5673032620530574</v>
       </c>
       <c r="AX119" s="25">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>16.98126691222053</v>
       </c>
       <c r="AY119" s="25">
-        <f t="shared" si="249"/>
+        <f t="shared" si="253"/>
         <v>24.376806374951329</v>
       </c>
     </row>

</xml_diff>